<commit_message>
get entities, synonyms e dialog nodes
</commit_message>
<xml_diff>
--- a/results/Perguntas.xlsx
+++ b/results/Perguntas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\Python\Filter-MSMARCO\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED687D05-90C8-4B64-8107-C438E05E8304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EB538B-BBBB-464C-A72D-4A9C7052C292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9972" yWindow="960" windowWidth="11820" windowHeight="10332" firstSheet="2" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="566" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="filtered_qna_manual_sorted" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8928" uniqueCount="2927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8926" uniqueCount="2930">
   <si>
     <t>query</t>
   </si>
@@ -8580,12 +8580,6 @@
     <t>Quais são as ameaças às tartarugas?</t>
   </si>
   <si>
-    <t>modificador</t>
-  </si>
-  <si>
-    <t>substantivo</t>
-  </si>
-  <si>
     <t>composicao</t>
   </si>
   <si>
@@ -8634,9 +8628,6 @@
     <t>tipos</t>
   </si>
   <si>
-    <t>recipiente</t>
-  </si>
-  <si>
     <t>iniciativas</t>
   </si>
   <si>
@@ -8661,9 +8652,6 @@
     <t>quantidade</t>
   </si>
   <si>
-    <t>brasil</t>
-  </si>
-  <si>
     <t>Qual é a maior reserva de petróleo no Brasil?</t>
   </si>
   <si>
@@ -8688,9 +8676,6 @@
     <t>quelonio</t>
   </si>
   <si>
-    <t>rótulos</t>
-  </si>
-  <si>
     <t>cagado</t>
   </si>
   <si>
@@ -8706,9 +8691,6 @@
     <t>nome</t>
   </si>
   <si>
-    <t>geral</t>
-  </si>
-  <si>
     <t>definir</t>
   </si>
   <si>
@@ -8821,6 +8803,33 @@
   </si>
   <si>
     <t>O que é energia de maré?</t>
+  </si>
+  <si>
+    <t>Rótulos</t>
+  </si>
+  <si>
+    <t>Modificador</t>
+  </si>
+  <si>
+    <t>Substantivo</t>
+  </si>
+  <si>
+    <t>Recipiente</t>
+  </si>
+  <si>
+    <t>maremoto</t>
+  </si>
+  <si>
+    <t>circulacao</t>
+  </si>
+  <si>
+    <t>trincheira-profunda</t>
+  </si>
+  <si>
+    <t>Como o oceano é usado?</t>
+  </si>
+  <si>
+    <t>acidificacao</t>
   </si>
 </sst>
 </file>
@@ -17907,7 +17916,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB571"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -30030,8 +30041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E933B6A1-031B-4D1D-8E81-FF5488950B7F}">
   <dimension ref="A1:AB571"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42188,8 +42199,8 @@
   <dimension ref="A1:AE502"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42198,10 +42209,10 @@
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" customWidth="1"/>
     <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="25.21875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="25.21875" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" customWidth="1"/>
     <col min="9" max="9" width="25.33203125" customWidth="1"/>
     <col min="28" max="28" width="8.88671875" customWidth="1"/>
   </cols>
@@ -42220,16 +42231,16 @@
         <v>2572</v>
       </c>
       <c r="E1" t="s">
-        <v>2882</v>
+        <v>2921</v>
       </c>
       <c r="F1" t="s">
-        <v>2846</v>
+        <v>2922</v>
       </c>
       <c r="G1" t="s">
-        <v>2847</v>
+        <v>2923</v>
       </c>
       <c r="H1" t="s">
-        <v>2864</v>
+        <v>2924</v>
       </c>
       <c r="I1" t="s">
         <v>2573</v>
@@ -42311,7 +42322,7 @@
         <v>coral-turismo</v>
       </c>
       <c r="F2" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="G2" t="s">
         <v>2708</v>
@@ -42340,10 +42351,10 @@
         <v>coral</v>
       </c>
       <c r="F3" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G3" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -42362,17 +42373,14 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>coral--definir-geral</v>
+        <v>coral--definir</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
         <v>coral</v>
       </c>
       <c r="F4" t="s">
-        <v>2889</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2888</v>
+        <v>2883</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -42398,7 +42406,7 @@
         <v>coral</v>
       </c>
       <c r="F5" t="s">
-        <v>2848</v>
+        <v>2846</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -42421,10 +42429,10 @@
         <v>coral</v>
       </c>
       <c r="F6" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G6" t="s">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -42447,10 +42455,10 @@
         <v>coral</v>
       </c>
       <c r="F7" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G7" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -42473,13 +42481,13 @@
         <v>coral</v>
       </c>
       <c r="F8" t="s">
+        <v>2851</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2862</v>
+      </c>
+      <c r="H8" t="s">
         <v>2853</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2865</v>
-      </c>
-      <c r="H8" t="s">
-        <v>2855</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -42502,10 +42510,10 @@
         <v>coral</v>
       </c>
       <c r="F9" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="G9" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -42528,10 +42536,10 @@
         <v>coral</v>
       </c>
       <c r="F10" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="H10" t="s">
-        <v>2863</v>
+        <v>2861</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -42554,10 +42562,10 @@
         <v>coral</v>
       </c>
       <c r="F11" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G11" t="s">
-        <v>2862</v>
+        <v>2860</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -42580,13 +42588,13 @@
         <v>coral</v>
       </c>
       <c r="F12" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="G12" t="s">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="H12" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -42632,10 +42640,10 @@
         <v>energia_de_mare</v>
       </c>
       <c r="F14" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="H14" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -42658,10 +42666,10 @@
         <v>energia_de_mare</v>
       </c>
       <c r="F15" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="H15" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -42673,7 +42681,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2923</v>
+        <v>2917</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -42684,10 +42692,10 @@
         <v>energia_de_mare</v>
       </c>
       <c r="F16" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G16" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -42699,7 +42707,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2924</v>
+        <v>2918</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -42710,10 +42718,10 @@
         <v>energia_de_mare</v>
       </c>
       <c r="F17" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G17" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -42725,7 +42733,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2925</v>
+        <v>2919</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -42736,10 +42744,10 @@
         <v>energia_de_mare</v>
       </c>
       <c r="F18" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G18" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -42762,7 +42770,7 @@
         <v>energia_de_mare</v>
       </c>
       <c r="F19" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -42778,20 +42786,17 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>energia_de_mare--definir-geral</v>
+        <v>energia_de_mare--definir</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="3"/>
         <v>energia_de_mare</v>
       </c>
       <c r="F20" t="s">
-        <v>2889</v>
-      </c>
-      <c r="H20" t="s">
-        <v>2888</v>
+        <v>2883</v>
       </c>
       <c r="I20" t="s">
-        <v>2926</v>
+        <v>2920</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -42814,10 +42819,10 @@
         <v>petroleo</v>
       </c>
       <c r="F21" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="G21" t="s">
-        <v>2866</v>
+        <v>2863</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -42939,20 +42944,17 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>petroleo--maiores-reserva-brasil</v>
+        <v>petroleo--maiores-reserva</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="3"/>
         <v>petroleo</v>
       </c>
       <c r="F27" t="s">
-        <v>2867</v>
+        <v>2864</v>
       </c>
       <c r="G27" t="s">
-        <v>2868</v>
-      </c>
-      <c r="H27" t="s">
-        <v>2873</v>
+        <v>2865</v>
       </c>
       <c r="L27">
         <v>1</v>
@@ -42964,24 +42966,21 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>2874</v>
+        <v>2870</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>petroleo--maior-reserva-brasil</v>
+        <v>petroleo--maior-reserva</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="3"/>
         <v>petroleo</v>
       </c>
       <c r="F28" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="G28" t="s">
-        <v>2868</v>
-      </c>
-      <c r="H28" t="s">
-        <v>2873</v>
+        <v>2865</v>
       </c>
       <c r="L28">
         <v>1</v>
@@ -43010,13 +43009,13 @@
         <v>petroleo</v>
       </c>
       <c r="F29" t="s">
+        <v>2864</v>
+      </c>
+      <c r="G29" t="s">
         <v>2867</v>
       </c>
-      <c r="G29" t="s">
-        <v>2870</v>
-      </c>
       <c r="H29" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
       <c r="L29">
         <v>1</v>
@@ -43045,13 +43044,13 @@
         <v>petroleo</v>
       </c>
       <c r="F30" t="s">
-        <v>2867</v>
+        <v>2864</v>
       </c>
       <c r="G30" t="s">
-        <v>2871</v>
+        <v>2868</v>
       </c>
       <c r="H30" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
       <c r="L30">
         <v>1</v>
@@ -43073,17 +43072,14 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>petroleo--quantidade-brasil</v>
+        <v>petroleo--quantidade</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="3"/>
         <v>petroleo</v>
       </c>
       <c r="F31" t="s">
-        <v>2872</v>
-      </c>
-      <c r="H31" t="s">
-        <v>2873</v>
+        <v>2869</v>
       </c>
       <c r="L31">
         <v>1</v>
@@ -43109,13 +43105,13 @@
         <v>petroleo</v>
       </c>
       <c r="F32" t="s">
-        <v>2872</v>
+        <v>2869</v>
       </c>
       <c r="G32" t="s">
-        <v>2871</v>
+        <v>2868</v>
       </c>
       <c r="H32" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -43261,7 +43257,7 @@
         <v>petroleo</v>
       </c>
       <c r="F39" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -43416,10 +43412,10 @@
         <v>petroleo</v>
       </c>
       <c r="F46" t="s">
-        <v>2872</v>
+        <v>2869</v>
       </c>
       <c r="H46" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
       <c r="L46">
         <v>1</v>
@@ -43448,10 +43444,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F47" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="H47" t="s">
-        <v>2877</v>
+        <v>2873</v>
       </c>
       <c r="M47">
         <v>1</v>
@@ -43500,10 +43496,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F49" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G49" t="s">
-        <v>2880</v>
+        <v>2876</v>
       </c>
       <c r="M49">
         <v>1</v>
@@ -43522,20 +43518,17 @@
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--diferenca-jabuti-tartaruga</v>
+        <v>tartaruga--diferenca-jabuti</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="3"/>
         <v>tartaruga</v>
       </c>
       <c r="F50" t="s">
-        <v>2878</v>
+        <v>2874</v>
       </c>
       <c r="G50" t="s">
-        <v>2876</v>
-      </c>
-      <c r="H50" t="s">
-        <v>2711</v>
+        <v>2872</v>
       </c>
       <c r="M50">
         <v>1</v>
@@ -43554,20 +43547,17 @@
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--pertence-jabuti-tartaruga</v>
+        <v>tartaruga--pertence-jabuti</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="3"/>
         <v>tartaruga</v>
       </c>
       <c r="F51" t="s">
-        <v>2879</v>
+        <v>2875</v>
       </c>
       <c r="G51" t="s">
-        <v>2876</v>
-      </c>
-      <c r="H51" t="s">
-        <v>2711</v>
+        <v>2872</v>
       </c>
       <c r="M51">
         <v>1</v>
@@ -43593,10 +43583,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F52" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G52" t="s">
-        <v>2881</v>
+        <v>2877</v>
       </c>
       <c r="M52">
         <v>1</v>
@@ -43622,10 +43612,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F53" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G53" t="s">
-        <v>2876</v>
+        <v>2872</v>
       </c>
       <c r="M53">
         <v>1</v>
@@ -43651,10 +43641,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F54" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G54" t="s">
-        <v>2883</v>
+        <v>2878</v>
       </c>
       <c r="M54">
         <v>1</v>
@@ -43673,17 +43663,14 @@
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--definir-geral</v>
+        <v>tartaruga--definir</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="3"/>
         <v>tartaruga</v>
       </c>
       <c r="F55" t="s">
-        <v>2889</v>
-      </c>
-      <c r="H55" t="s">
-        <v>2888</v>
+        <v>2883</v>
       </c>
       <c r="M55">
         <v>1</v>
@@ -43732,13 +43719,13 @@
         <v>tartaruga</v>
       </c>
       <c r="F57" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G57" t="s">
-        <v>2880</v>
+        <v>2876</v>
       </c>
       <c r="H57" t="s">
-        <v>2884</v>
+        <v>2879</v>
       </c>
       <c r="M57">
         <v>1</v>
@@ -43764,10 +43751,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F58" t="s">
-        <v>2885</v>
+        <v>2880</v>
       </c>
       <c r="H58" t="s">
-        <v>2884</v>
+        <v>2879</v>
       </c>
       <c r="I58" t="s">
         <v>2845</v>
@@ -43876,10 +43863,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F63" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G63" t="s">
-        <v>2886</v>
+        <v>2881</v>
       </c>
       <c r="M63">
         <v>1</v>
@@ -43965,7 +43952,7 @@
         <v>tartaruga</v>
       </c>
       <c r="F67" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="M67">
         <v>1</v>
@@ -44034,10 +44021,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F70" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G70" t="s">
-        <v>2875</v>
+        <v>2871</v>
       </c>
       <c r="M70">
         <v>1</v>
@@ -44595,7 +44582,7 @@
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
-        <v>1224</v>
+        <v>2928</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="4"/>
@@ -44619,12 +44606,18 @@
       </c>
       <c r="D99" t="str">
         <f t="shared" si="4"/>
-        <v>oceano</v>
+        <v>oceano--motivo-circulacao</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="6"/>
         <v>oceano</v>
       </c>
+      <c r="F99" t="s">
+        <v>2880</v>
+      </c>
+      <c r="G99" t="s">
+        <v>2926</v>
+      </c>
       <c r="O99">
         <v>1</v>
       </c>
@@ -44639,13 +44632,19 @@
       </c>
       <c r="D100" t="str">
         <f t="shared" si="4"/>
-        <v>oceano</v>
+        <v>extra--definir-trincheira-profunda</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="6"/>
-        <v>oceano</v>
-      </c>
-      <c r="O100">
+        <v>extra</v>
+      </c>
+      <c r="F100" t="s">
+        <v>2883</v>
+      </c>
+      <c r="G100" t="s">
+        <v>2927</v>
+      </c>
+      <c r="AD100">
         <v>1</v>
       </c>
       <c r="AE100">
@@ -44679,12 +44678,18 @@
       </c>
       <c r="D102" t="str">
         <f t="shared" si="4"/>
-        <v>oceano</v>
+        <v>oceano--definir-acidificacao</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="6"/>
         <v>oceano</v>
       </c>
+      <c r="F102" t="s">
+        <v>2883</v>
+      </c>
+      <c r="G102" t="s">
+        <v>2929</v>
+      </c>
       <c r="O102">
         <v>1</v>
       </c>
@@ -45085,12 +45090,15 @@
       </c>
       <c r="D122" t="str">
         <f t="shared" si="4"/>
-        <v>mare</v>
+        <v>mare--motivo</v>
       </c>
       <c r="E122" t="str">
         <f t="shared" si="6"/>
         <v>mare</v>
       </c>
+      <c r="F122" t="s">
+        <v>2880</v>
+      </c>
       <c r="Q122">
         <v>1</v>
       </c>
@@ -45105,13 +45113,19 @@
       </c>
       <c r="D123" t="str">
         <f t="shared" si="4"/>
-        <v>mare</v>
+        <v>extra--definir-maremoto</v>
       </c>
       <c r="E123" t="str">
         <f t="shared" si="6"/>
-        <v>mare</v>
-      </c>
-      <c r="Q123">
+        <v>extra</v>
+      </c>
+      <c r="F123" t="s">
+        <v>2883</v>
+      </c>
+      <c r="G123" t="s">
+        <v>2925</v>
+      </c>
+      <c r="AD123">
         <v>1</v>
       </c>
       <c r="AE123">
@@ -45325,13 +45339,13 @@
       </c>
       <c r="D134" t="str">
         <f t="shared" si="8"/>
-        <v>navio</v>
+        <v>extra</v>
       </c>
       <c r="E134" t="str">
         <f t="shared" si="6"/>
-        <v>navio</v>
-      </c>
-      <c r="T134">
+        <v>extra</v>
+      </c>
+      <c r="AD134">
         <v>1</v>
       </c>
       <c r="AE134">
@@ -45345,13 +45359,13 @@
       </c>
       <c r="D135" t="str">
         <f t="shared" si="8"/>
-        <v>navio</v>
+        <v>extra</v>
       </c>
       <c r="E135" t="str">
         <f t="shared" si="6"/>
-        <v>navio</v>
-      </c>
-      <c r="T135">
+        <v>extra</v>
+      </c>
+      <c r="AD135">
         <v>1</v>
       </c>
       <c r="AE135">
@@ -45464,10 +45478,10 @@
         <v>flora</v>
       </c>
       <c r="F140" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G140" t="s">
-        <v>2890</v>
+        <v>2884</v>
       </c>
       <c r="U140">
         <v>1</v>
@@ -45496,10 +45510,10 @@
         <v>flora-fauna</v>
       </c>
       <c r="F141" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G141" t="s">
-        <v>2892</v>
+        <v>2886</v>
       </c>
       <c r="U141">
         <v>1</v>
@@ -45531,10 +45545,10 @@
         <v>flora-fauna</v>
       </c>
       <c r="F142" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G142" t="s">
-        <v>2893</v>
+        <v>2887</v>
       </c>
       <c r="U142">
         <v>1</v>
@@ -45566,10 +45580,10 @@
         <v>fauna</v>
       </c>
       <c r="F143" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G143" t="s">
-        <v>2894</v>
+        <v>2888</v>
       </c>
       <c r="V143">
         <v>1</v>
@@ -45598,13 +45612,13 @@
         <v>fauna</v>
       </c>
       <c r="F144" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G144" t="s">
         <v>2708</v>
       </c>
       <c r="H144" t="s">
-        <v>2877</v>
+        <v>2873</v>
       </c>
       <c r="V144">
         <v>1</v>
@@ -45630,10 +45644,10 @@
         <v>fauna</v>
       </c>
       <c r="F145" t="s">
+        <v>2883</v>
+      </c>
+      <c r="G145" t="s">
         <v>2889</v>
-      </c>
-      <c r="G145" t="s">
-        <v>2895</v>
       </c>
       <c r="V145">
         <v>1</v>
@@ -45659,13 +45673,13 @@
         <v>fauna</v>
       </c>
       <c r="F146" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G146" t="s">
-        <v>2899</v>
+        <v>2893</v>
       </c>
       <c r="H146" t="s">
-        <v>2891</v>
+        <v>2885</v>
       </c>
       <c r="V146">
         <v>1</v>
@@ -45691,13 +45705,13 @@
         <v>fauna</v>
       </c>
       <c r="F147" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G147" t="s">
-        <v>2899</v>
+        <v>2893</v>
       </c>
       <c r="H147" t="s">
-        <v>2891</v>
+        <v>2885</v>
       </c>
       <c r="V147">
         <v>1</v>
@@ -45726,10 +45740,10 @@
         <v>fauna</v>
       </c>
       <c r="F148" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G148" t="s">
-        <v>2896</v>
+        <v>2890</v>
       </c>
       <c r="V148">
         <v>1</v>
@@ -45758,10 +45772,10 @@
         <v>fauna</v>
       </c>
       <c r="F149" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G149" t="s">
-        <v>2902</v>
+        <v>2896</v>
       </c>
       <c r="V149">
         <v>1</v>
@@ -45790,10 +45804,10 @@
         <v>fauna</v>
       </c>
       <c r="F150" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G150" t="s">
-        <v>2903</v>
+        <v>2897</v>
       </c>
       <c r="V150">
         <v>1</v>
@@ -45805,7 +45819,7 @@
     </row>
     <row r="151" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
-        <v>2919</v>
+        <v>2913</v>
       </c>
       <c r="D151" t="str">
         <f t="shared" si="8"/>
@@ -45816,13 +45830,13 @@
         <v>fauna</v>
       </c>
       <c r="F151" t="s">
-        <v>2879</v>
+        <v>2875</v>
       </c>
       <c r="G151" t="s">
-        <v>2903</v>
+        <v>2897</v>
       </c>
       <c r="H151" t="s">
-        <v>2896</v>
+        <v>2890</v>
       </c>
       <c r="V151">
         <v>1</v>
@@ -45851,13 +45865,13 @@
         <v>fauna</v>
       </c>
       <c r="F152" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="G152" t="s">
-        <v>2899</v>
+        <v>2893</v>
       </c>
       <c r="H152" t="s">
-        <v>2891</v>
+        <v>2885</v>
       </c>
       <c r="V152">
         <v>1</v>
@@ -45876,20 +45890,17 @@
       </c>
       <c r="D153" t="str">
         <f t="shared" si="8"/>
-        <v>fauna--existe-baleia-brasil</v>
+        <v>fauna--existe-baleia</v>
       </c>
       <c r="E153" t="str">
         <f t="shared" si="9"/>
         <v>fauna</v>
       </c>
       <c r="F153" t="s">
-        <v>2904</v>
+        <v>2898</v>
       </c>
       <c r="G153" t="s">
-        <v>2905</v>
-      </c>
-      <c r="H153" t="s">
-        <v>2873</v>
+        <v>2899</v>
       </c>
       <c r="V153">
         <v>1</v>
@@ -45911,20 +45922,17 @@
       </c>
       <c r="D154" t="str">
         <f t="shared" si="8"/>
-        <v>fauna-turismo--localizacao-baleia-brasil</v>
+        <v>fauna-turismo--localizacao-baleia</v>
       </c>
       <c r="E154" t="str">
         <f t="shared" si="9"/>
         <v>fauna-turismo</v>
       </c>
       <c r="F154" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="G154" t="s">
-        <v>2905</v>
-      </c>
-      <c r="H154" t="s">
-        <v>2873</v>
+        <v>2899</v>
       </c>
       <c r="V154">
         <v>1</v>
@@ -46016,10 +46024,10 @@
         <v>fauna</v>
       </c>
       <c r="F158" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G158" t="s">
-        <v>2906</v>
+        <v>2900</v>
       </c>
       <c r="V158">
         <v>1</v>
@@ -46048,10 +46056,10 @@
         <v>fauna</v>
       </c>
       <c r="F159" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G159" t="s">
-        <v>2907</v>
+        <v>2901</v>
       </c>
       <c r="V159">
         <v>1</v>
@@ -46077,10 +46085,10 @@
         <v>fauna</v>
       </c>
       <c r="F160" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G160" t="s">
-        <v>2897</v>
+        <v>2891</v>
       </c>
       <c r="V160">
         <v>1</v>
@@ -46109,10 +46117,10 @@
         <v>fauna</v>
       </c>
       <c r="F161" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G161" t="s">
-        <v>2908</v>
+        <v>2902</v>
       </c>
       <c r="V161">
         <v>1</v>
@@ -46141,10 +46149,10 @@
         <v>fauna</v>
       </c>
       <c r="F162" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G162" t="s">
-        <v>2909</v>
+        <v>2903</v>
       </c>
       <c r="V162">
         <v>1</v>
@@ -46170,10 +46178,10 @@
         <v>fauna</v>
       </c>
       <c r="F163" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G163" t="s">
-        <v>2898</v>
+        <v>2892</v>
       </c>
       <c r="V163">
         <v>1</v>
@@ -46195,20 +46203,17 @@
       </c>
       <c r="D164" t="str">
         <f t="shared" si="8"/>
-        <v>fauna-turismo--existe-tubarao-brasil</v>
+        <v>fauna-turismo--existe-tubarao</v>
       </c>
       <c r="E164" t="str">
         <f t="shared" si="9"/>
         <v>fauna-turismo</v>
       </c>
       <c r="F164" t="s">
-        <v>2904</v>
+        <v>2898</v>
       </c>
       <c r="G164" t="s">
-        <v>2903</v>
-      </c>
-      <c r="H164" t="s">
-        <v>2873</v>
+        <v>2897</v>
       </c>
       <c r="V164">
         <v>1</v>
@@ -46257,10 +46262,10 @@
         <v>fauna</v>
       </c>
       <c r="F166" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G166" t="s">
-        <v>2912</v>
+        <v>2906</v>
       </c>
       <c r="V166">
         <v>1</v>
@@ -46289,10 +46294,10 @@
         <v>fauna</v>
       </c>
       <c r="F167" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G167" t="s">
-        <v>2900</v>
+        <v>2894</v>
       </c>
       <c r="V167">
         <v>1</v>
@@ -46318,10 +46323,10 @@
         <v>fauna</v>
       </c>
       <c r="F168" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G168" t="s">
-        <v>2901</v>
+        <v>2895</v>
       </c>
       <c r="V168">
         <v>1</v>
@@ -46347,10 +46352,10 @@
         <v>fauna</v>
       </c>
       <c r="F169" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G169" t="s">
-        <v>2901</v>
+        <v>2895</v>
       </c>
       <c r="V169">
         <v>1</v>
@@ -46399,10 +46404,10 @@
         <v>fauna</v>
       </c>
       <c r="F171" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G171" t="s">
-        <v>2912</v>
+        <v>2906</v>
       </c>
       <c r="V171">
         <v>1</v>
@@ -46428,10 +46433,10 @@
         <v>fauna</v>
       </c>
       <c r="F172" t="s">
-        <v>2913</v>
+        <v>2907</v>
       </c>
       <c r="G172" t="s">
-        <v>2912</v>
+        <v>2906</v>
       </c>
       <c r="V172">
         <v>1</v>
@@ -46460,10 +46465,10 @@
         <v>fauna</v>
       </c>
       <c r="F173" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G173" t="s">
-        <v>2910</v>
+        <v>2904</v>
       </c>
       <c r="V173">
         <v>1</v>
@@ -46492,13 +46497,13 @@
         <v>fauna</v>
       </c>
       <c r="F174" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G174" t="s">
-        <v>2914</v>
+        <v>2908</v>
       </c>
       <c r="I174" t="s">
-        <v>2915</v>
+        <v>2909</v>
       </c>
       <c r="V174">
         <v>1</v>
@@ -46527,10 +46532,10 @@
         <v>fauna</v>
       </c>
       <c r="F175" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G175" t="s">
-        <v>2916</v>
+        <v>2910</v>
       </c>
       <c r="V175">
         <v>1</v>
@@ -46545,7 +46550,7 @@
         <v>2768</v>
       </c>
       <c r="B176" t="s">
-        <v>2918</v>
+        <v>2912</v>
       </c>
       <c r="C176" t="s">
         <v>2769</v>
@@ -46559,13 +46564,13 @@
         <v>fauna</v>
       </c>
       <c r="F176" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G176" t="s">
+        <v>2905</v>
+      </c>
+      <c r="I176" t="s">
         <v>2911</v>
-      </c>
-      <c r="I176" t="s">
-        <v>2917</v>
       </c>
       <c r="V176">
         <v>1</v>
@@ -46591,10 +46596,10 @@
         <v>fauna</v>
       </c>
       <c r="F177" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G177" t="s">
-        <v>2916</v>
+        <v>2910</v>
       </c>
       <c r="V177">
         <v>1</v>
@@ -47183,13 +47188,13 @@
         <v>extra</v>
       </c>
       <c r="F206" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
       <c r="G206" t="s">
-        <v>2871</v>
+        <v>2868</v>
       </c>
       <c r="H206" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
       <c r="AD206">
         <v>1</v>
@@ -47212,13 +47217,13 @@
         <v>extra</v>
       </c>
       <c r="F207" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="G207" t="s">
-        <v>2922</v>
+        <v>2916</v>
       </c>
       <c r="H207" t="s">
-        <v>2921</v>
+        <v>2915</v>
       </c>
       <c r="AD207">
         <v>1</v>
@@ -47247,13 +47252,13 @@
         <v>extra</v>
       </c>
       <c r="F208" t="s">
-        <v>2885</v>
+        <v>2880</v>
       </c>
       <c r="G208" t="s">
-        <v>2920</v>
+        <v>2914</v>
       </c>
       <c r="H208" t="s">
-        <v>2921</v>
+        <v>2915</v>
       </c>
       <c r="AD208">
         <v>1</v>
@@ -47282,13 +47287,13 @@
         <v>extra</v>
       </c>
       <c r="F209" t="s">
-        <v>2885</v>
+        <v>2880</v>
       </c>
       <c r="G209" t="s">
-        <v>2887</v>
+        <v>2882</v>
       </c>
       <c r="H209" t="s">
-        <v>2921</v>
+        <v>2915</v>
       </c>
       <c r="AD209">
         <v>1</v>

</xml_diff>

<commit_message>
limpa output do notebook
</commit_message>
<xml_diff>
--- a/results/Perguntas.xlsx
+++ b/results/Perguntas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\Python\Filter-MSMARCO\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B16DAB-DABD-4D0A-8DAF-256DF4C7E0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA3BDC-C70D-44E7-93C4-57FDF0F7D493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9972" yWindow="960" windowWidth="11820" windowHeight="10332" tabRatio="566" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
+    <workbookView xWindow="17175" yWindow="-14730" windowWidth="11820" windowHeight="10335" tabRatio="566" firstSheet="2" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="filtered_qna_manual_sorted" sheetId="1" r:id="rId1"/>
@@ -42201,16 +42201,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17344D9D-8D84-42DD-9996-E6496156E107}">
   <dimension ref="A1:AF502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="125.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.77734375" customWidth="1"/>
     <col min="6" max="6" width="17.21875" customWidth="1"/>

</xml_diff>

<commit_message>
fix pergunta com erro
</commit_message>
<xml_diff>
--- a/results/Perguntas.xlsx
+++ b/results/Perguntas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\Python\Filter-MSMARCO\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA3BDC-C70D-44E7-93C4-57FDF0F7D493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F09AF60-BEE8-47F6-99AE-F39B52D565FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17175" yWindow="-14730" windowWidth="11820" windowHeight="10335" tabRatio="566" firstSheet="2" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8928" uniqueCount="2931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8927" uniqueCount="2930">
   <si>
     <t>query</t>
   </si>
@@ -8428,9 +8428,6 @@
   </si>
   <si>
     <t>O petróleo fica em bolsões profundos na terra, nas chamadas bacias sedimentares. Ele fica retido em pedras porosas, que, por sua vez, precisam ser cercadas de pedras impermeáveis para que ele não escape.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Animais marinhos são aqueles que vivem no mar. É importante distinguí-los de animais de água doce, que vivem, por exemplo, em rios. Ambos são aquáticos.</t>
@@ -42202,14 +42199,14 @@
   <dimension ref="A1:AF502"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="2" max="2" width="125.6640625" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.77734375" customWidth="1"/>
@@ -42234,16 +42231,16 @@
         <v>2572</v>
       </c>
       <c r="E1" t="s">
+        <v>2896</v>
+      </c>
+      <c r="F1" t="s">
         <v>2897</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2898</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2899</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2900</v>
       </c>
       <c r="I1" t="s">
         <v>2573</v>
@@ -42252,19 +42249,19 @@
         <v>2708</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>2911</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>2912</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>2913</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>2709</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>2710</v>
@@ -42273,10 +42270,10 @@
         <v>2711</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>2712</v>
@@ -42328,7 +42325,7 @@
         <v>coral-turismo</v>
       </c>
       <c r="F2" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="G2" t="s">
         <v>2717</v>
@@ -42360,10 +42357,10 @@
         <v>coral</v>
       </c>
       <c r="F3" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G3" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -42389,7 +42386,7 @@
         <v>coral</v>
       </c>
       <c r="F4" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -42415,7 +42412,7 @@
         <v>coral</v>
       </c>
       <c r="F5" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -42438,10 +42435,10 @@
         <v>coral</v>
       </c>
       <c r="F6" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G6" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -42464,10 +42461,10 @@
         <v>coral</v>
       </c>
       <c r="F7" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G7" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -42490,13 +42487,13 @@
         <v>coral</v>
       </c>
       <c r="F8" t="s">
+        <v>2843</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2851</v>
+      </c>
+      <c r="H8" t="s">
         <v>2844</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2852</v>
-      </c>
-      <c r="H8" t="s">
-        <v>2845</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -42519,10 +42516,10 @@
         <v>coral</v>
       </c>
       <c r="F9" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="G9" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -42545,10 +42542,10 @@
         <v>coral</v>
       </c>
       <c r="F10" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="H10" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -42571,10 +42568,10 @@
         <v>coral</v>
       </c>
       <c r="F11" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G11" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -42597,13 +42594,13 @@
         <v>coral</v>
       </c>
       <c r="F12" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="G12" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="H12" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -42649,13 +42646,13 @@
         <v>energia_de_maré</v>
       </c>
       <c r="F14" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="G14" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
       <c r="H14" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -42678,13 +42675,13 @@
         <v>energia_de_maré</v>
       </c>
       <c r="F15" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="G15" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
       <c r="H15" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -42696,7 +42693,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -42707,10 +42704,10 @@
         <v>energia_de_maré</v>
       </c>
       <c r="F16" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G16" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -42722,7 +42719,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -42733,10 +42730,10 @@
         <v>energia_de_maré</v>
       </c>
       <c r="F17" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G17" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -42748,7 +42745,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -42759,10 +42756,10 @@
         <v>energia_de_maré</v>
       </c>
       <c r="F18" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G18" t="s">
-        <v>2929</v>
+        <v>2928</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -42785,7 +42782,7 @@
         <v>energia_de_maré</v>
       </c>
       <c r="F19" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -42808,10 +42805,10 @@
         <v>energia_de_maré</v>
       </c>
       <c r="F20" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="I20" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -42834,10 +42831,10 @@
         <v>petróleo</v>
       </c>
       <c r="F21" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G21" t="s">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -42966,10 +42963,10 @@
         <v>petróleo</v>
       </c>
       <c r="F27" t="s">
+        <v>2853</v>
+      </c>
+      <c r="G27" t="s">
         <v>2854</v>
-      </c>
-      <c r="G27" t="s">
-        <v>2855</v>
       </c>
       <c r="L27">
         <v>1</v>
@@ -42981,7 +42978,7 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>2858</v>
+        <v>2857</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -42992,10 +42989,10 @@
         <v>petróleo</v>
       </c>
       <c r="F28" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G28" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="L28">
         <v>1</v>
@@ -43024,13 +43021,13 @@
         <v>gás</v>
       </c>
       <c r="F29" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="G29" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="H29" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -43059,13 +43056,13 @@
         <v>petróleo</v>
       </c>
       <c r="F30" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="G30" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="H30" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="L30">
         <v>1</v>
@@ -43094,7 +43091,7 @@
         <v>petróleo</v>
       </c>
       <c r="F31" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="L31">
         <v>1</v>
@@ -43120,10 +43117,10 @@
         <v>gás</v>
       </c>
       <c r="F32" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="H32" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -43272,7 +43269,7 @@
         <v>petróleo</v>
       </c>
       <c r="F39" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -43286,9 +43283,6 @@
       <c r="A40" t="s">
         <v>2616</v>
       </c>
-      <c r="B40" t="s">
-        <v>2796</v>
-      </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
         <v>petróleo</v>
@@ -43427,10 +43421,10 @@
         <v>petróleo</v>
       </c>
       <c r="F46" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="H46" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="L46">
         <v>1</v>
@@ -43459,10 +43453,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F47" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="H47" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="N47">
         <v>1</v>
@@ -43500,7 +43494,7 @@
         <v>2576</v>
       </c>
       <c r="B49" t="s">
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
@@ -43511,10 +43505,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F49" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G49" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="N49">
         <v>1</v>
@@ -43529,7 +43523,7 @@
         <v>2577</v>
       </c>
       <c r="B50" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
@@ -43540,10 +43534,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F50" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="G50" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="N50">
         <v>1</v>
@@ -43569,10 +43563,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F51" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="G51" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -43598,10 +43592,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F52" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G52" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="N52">
         <v>1</v>
@@ -43616,7 +43610,7 @@
         <v>2578</v>
       </c>
       <c r="B53" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
@@ -43627,10 +43621,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F53" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G53" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -43645,7 +43639,7 @@
         <v>2579</v>
       </c>
       <c r="B54" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
@@ -43656,10 +43650,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F54" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G54" t="s">
-        <v>2927</v>
+        <v>2926</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -43674,7 +43668,7 @@
         <v>2580</v>
       </c>
       <c r="B55" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
@@ -43685,7 +43679,7 @@
         <v>tartaruga</v>
       </c>
       <c r="F55" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -43720,10 +43714,10 @@
         <v>2582</v>
       </c>
       <c r="B57" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="C57" t="s">
-        <v>2831</v>
+        <v>2830</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
@@ -43734,13 +43728,13 @@
         <v>tartaruga</v>
       </c>
       <c r="F57" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G57" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="H57" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="N57">
         <v>1</v>
@@ -43752,10 +43746,10 @@
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>2836</v>
+      </c>
+      <c r="B58" t="s">
         <v>2837</v>
-      </c>
-      <c r="B58" t="s">
-        <v>2838</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
@@ -43766,13 +43760,13 @@
         <v>tartaruga</v>
       </c>
       <c r="F58" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="H58" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="I58" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -43867,7 +43861,7 @@
         <v>2587</v>
       </c>
       <c r="B63" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
@@ -43878,10 +43872,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F63" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G63" t="s">
-        <v>2864</v>
+        <v>2863</v>
       </c>
       <c r="N63">
         <v>1</v>
@@ -43956,7 +43950,7 @@
         <v>2591</v>
       </c>
       <c r="B67" t="s">
-        <v>2829</v>
+        <v>2828</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="4"/>
@@ -43967,7 +43961,7 @@
         <v>tartaruga</v>
       </c>
       <c r="F67" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="N67">
         <v>1</v>
@@ -44036,10 +44030,10 @@
         <v>tartaruga</v>
       </c>
       <c r="F70" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G70" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="N70">
         <v>1</v>
@@ -44597,7 +44591,7 @@
     </row>
     <row r="98" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="4"/>
@@ -44628,10 +44622,10 @@
         <v>oceano</v>
       </c>
       <c r="F99" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="G99" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="P99">
         <v>1</v>
@@ -44654,10 +44648,10 @@
         <v>extra</v>
       </c>
       <c r="F100" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G100" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="AE100">
         <v>1</v>
@@ -44700,10 +44694,10 @@
         <v>oceano</v>
       </c>
       <c r="F102" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G102" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="P102">
         <v>1</v>
@@ -45112,7 +45106,7 @@
         <v>maré</v>
       </c>
       <c r="F122" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="R122">
         <v>1</v>
@@ -45135,10 +45129,10 @@
         <v>extra</v>
       </c>
       <c r="F123" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G123" t="s">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="AE123">
         <v>1</v>
@@ -45479,10 +45473,10 @@
         <v>2706</v>
       </c>
       <c r="B140" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="C140" t="s">
-        <v>2822</v>
+        <v>2821</v>
       </c>
       <c r="D140" t="str">
         <f t="shared" si="8"/>
@@ -45493,10 +45487,10 @@
         <v>flora</v>
       </c>
       <c r="F140" t="s">
+        <v>2865</v>
+      </c>
+      <c r="G140" t="s">
         <v>2866</v>
-      </c>
-      <c r="G140" t="s">
-        <v>2867</v>
       </c>
       <c r="V140">
         <v>1</v>
@@ -45508,13 +45502,13 @@
     </row>
     <row r="141" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
-        <v>2818</v>
+        <v>2817</v>
       </c>
       <c r="B141" t="s">
+        <v>2822</v>
+      </c>
+      <c r="C141" t="s">
         <v>2823</v>
-      </c>
-      <c r="C141" t="s">
-        <v>2824</v>
       </c>
       <c r="D141" t="str">
         <f t="shared" si="8"/>
@@ -45525,10 +45519,10 @@
         <v>flora-fauna</v>
       </c>
       <c r="F141" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G141" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="V141">
         <v>1</v>
@@ -45543,13 +45537,13 @@
     </row>
     <row r="142" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
+        <v>2818</v>
+      </c>
+      <c r="B142" t="s">
+        <v>2820</v>
+      </c>
+      <c r="C142" t="s">
         <v>2819</v>
-      </c>
-      <c r="B142" t="s">
-        <v>2821</v>
-      </c>
-      <c r="C142" t="s">
-        <v>2820</v>
       </c>
       <c r="D142" t="str">
         <f t="shared" si="8"/>
@@ -45560,10 +45554,10 @@
         <v>flora-fauna</v>
       </c>
       <c r="F142" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G142" t="s">
-        <v>2921</v>
+        <v>2920</v>
       </c>
       <c r="V142">
         <v>1</v>
@@ -45595,10 +45589,10 @@
         <v>fauna</v>
       </c>
       <c r="F143" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G143" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="W143">
         <v>1</v>
@@ -45627,13 +45621,13 @@
         <v>fauna</v>
       </c>
       <c r="F144" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G144" t="s">
         <v>2708</v>
       </c>
       <c r="H144" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="W144">
         <v>1</v>
@@ -45659,10 +45653,10 @@
         <v>fauna</v>
       </c>
       <c r="F145" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G145" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="W145">
         <v>1</v>
@@ -45674,10 +45668,10 @@
     </row>
     <row r="146" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A146" s="7" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="B146" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="D146" t="str">
         <f t="shared" si="8"/>
@@ -45688,13 +45682,13 @@
         <v>fauna</v>
       </c>
       <c r="F146" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G146" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
       <c r="H146" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="W146">
         <v>1</v>
@@ -45706,10 +45700,10 @@
     </row>
     <row r="147" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="B147" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="D147" t="str">
         <f t="shared" si="8"/>
@@ -45720,13 +45714,13 @@
         <v>fauna</v>
       </c>
       <c r="F147" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G147" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
       <c r="H147" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="W147">
         <v>1</v>
@@ -45738,13 +45732,13 @@
     </row>
     <row r="148" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A148" s="7" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="B148" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="C148" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="D148" t="str">
         <f t="shared" si="8"/>
@@ -45755,10 +45749,10 @@
         <v>fauna</v>
       </c>
       <c r="F148" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G148" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="W148">
         <v>1</v>
@@ -45770,13 +45764,13 @@
     </row>
     <row r="149" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
+        <v>2801</v>
+      </c>
+      <c r="B149" t="s">
         <v>2802</v>
       </c>
-      <c r="B149" t="s">
-        <v>2803</v>
-      </c>
       <c r="C149" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="D149" t="str">
         <f t="shared" si="8"/>
@@ -45787,10 +45781,10 @@
         <v>fauna</v>
       </c>
       <c r="F149" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G149" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="W149">
         <v>1</v>
@@ -45802,13 +45796,13 @@
     </row>
     <row r="150" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A150" s="7" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="B150" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="C150" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="D150" t="str">
         <f t="shared" si="8"/>
@@ -45819,10 +45813,10 @@
         <v>fauna</v>
       </c>
       <c r="F150" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G150" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="W150">
         <v>1</v>
@@ -45834,7 +45828,7 @@
     </row>
     <row r="151" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
       <c r="D151" t="str">
         <f t="shared" si="8"/>
@@ -45845,13 +45839,13 @@
         <v>fauna</v>
       </c>
       <c r="F151" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="G151" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="H151" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="W151">
         <v>1</v>
@@ -45866,10 +45860,10 @@
         <v>2679</v>
       </c>
       <c r="B152" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="C152" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="8"/>
@@ -45880,13 +45874,13 @@
         <v>fauna</v>
       </c>
       <c r="F152" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G152" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
       <c r="H152" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="W152">
         <v>1</v>
@@ -45898,10 +45892,10 @@
     </row>
     <row r="153" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="B153" t="s">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="D153" t="str">
         <f t="shared" si="8"/>
@@ -45912,10 +45906,10 @@
         <v>fauna</v>
       </c>
       <c r="F153" t="s">
+        <v>2876</v>
+      </c>
+      <c r="G153" t="s">
         <v>2877</v>
-      </c>
-      <c r="G153" t="s">
-        <v>2878</v>
       </c>
       <c r="W153">
         <v>1</v>
@@ -45927,13 +45921,13 @@
     </row>
     <row r="154" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
+        <v>2814</v>
+      </c>
+      <c r="B154" t="s">
+        <v>2816</v>
+      </c>
+      <c r="C154" t="s">
         <v>2815</v>
-      </c>
-      <c r="B154" t="s">
-        <v>2817</v>
-      </c>
-      <c r="C154" t="s">
-        <v>2816</v>
       </c>
       <c r="D154" t="str">
         <f t="shared" si="8"/>
@@ -45944,10 +45938,10 @@
         <v>fauna-turismo</v>
       </c>
       <c r="F154" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="G154" t="s">
-        <v>2878</v>
+        <v>2877</v>
       </c>
       <c r="W154">
         <v>1</v>
@@ -46025,7 +46019,7 @@
         <v>2683</v>
       </c>
       <c r="B158" t="s">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="C158" t="s">
         <v>2759</v>
@@ -46039,10 +46033,10 @@
         <v>fauna</v>
       </c>
       <c r="F158" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G158" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
       <c r="W158">
         <v>1</v>
@@ -46057,7 +46051,7 @@
         <v>2772</v>
       </c>
       <c r="B159" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="C159" t="s">
         <v>2774</v>
@@ -46071,10 +46065,10 @@
         <v>fauna</v>
       </c>
       <c r="F159" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G159" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="W159">
         <v>1</v>
@@ -46100,10 +46094,10 @@
         <v>fauna</v>
       </c>
       <c r="F160" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G160" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="W160">
         <v>1</v>
@@ -46118,7 +46112,7 @@
         <v>2773</v>
       </c>
       <c r="B161" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="C161" t="s">
         <v>2775</v>
@@ -46132,10 +46126,10 @@
         <v>fauna</v>
       </c>
       <c r="F161" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G161" t="s">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="W161">
         <v>1</v>
@@ -46164,10 +46158,10 @@
         <v>fauna</v>
       </c>
       <c r="F162" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G162" t="s">
-        <v>2882</v>
+        <v>2881</v>
       </c>
       <c r="W162">
         <v>1</v>
@@ -46193,10 +46187,10 @@
         <v>fauna</v>
       </c>
       <c r="F163" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G163" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
       <c r="W163">
         <v>1</v>
@@ -46211,10 +46205,10 @@
         <v>2685</v>
       </c>
       <c r="B164" t="s">
+        <v>2804</v>
+      </c>
+      <c r="C164" t="s">
         <v>2805</v>
-      </c>
-      <c r="C164" t="s">
-        <v>2806</v>
       </c>
       <c r="D164" t="str">
         <f t="shared" si="8"/>
@@ -46225,10 +46219,10 @@
         <v>fauna-turismo</v>
       </c>
       <c r="F164" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="G164" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="W164">
         <v>1</v>
@@ -46277,10 +46271,10 @@
         <v>fauna</v>
       </c>
       <c r="F166" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G166" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="W166">
         <v>1</v>
@@ -46309,10 +46303,10 @@
         <v>fauna</v>
       </c>
       <c r="F167" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G167" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="W167">
         <v>1</v>
@@ -46338,10 +46332,10 @@
         <v>fauna</v>
       </c>
       <c r="F168" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G168" t="s">
-        <v>2876</v>
+        <v>2875</v>
       </c>
       <c r="W168">
         <v>1</v>
@@ -46367,10 +46361,10 @@
         <v>fauna</v>
       </c>
       <c r="F169" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G169" t="s">
-        <v>2876</v>
+        <v>2875</v>
       </c>
       <c r="W169">
         <v>1</v>
@@ -46419,10 +46413,10 @@
         <v>fauna</v>
       </c>
       <c r="F171" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G171" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="W171">
         <v>1</v>
@@ -46448,10 +46442,10 @@
         <v>fauna</v>
       </c>
       <c r="F172" t="s">
-        <v>2885</v>
+        <v>2884</v>
       </c>
       <c r="G172" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="W172">
         <v>1</v>
@@ -46480,10 +46474,10 @@
         <v>fauna</v>
       </c>
       <c r="F173" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G173" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="W173">
         <v>1</v>
@@ -46512,13 +46506,13 @@
         <v>fauna</v>
       </c>
       <c r="F174" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G174" t="s">
+        <v>2885</v>
+      </c>
+      <c r="I174" t="s">
         <v>2886</v>
-      </c>
-      <c r="I174" t="s">
-        <v>2887</v>
       </c>
       <c r="W174">
         <v>1</v>
@@ -46547,10 +46541,10 @@
         <v>fauna</v>
       </c>
       <c r="F175" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G175" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="W175">
         <v>1</v>
@@ -46565,7 +46559,7 @@
         <v>2763</v>
       </c>
       <c r="B176" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
       <c r="C176" t="s">
         <v>2764</v>
@@ -46579,13 +46573,13 @@
         <v>fauna</v>
       </c>
       <c r="F176" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="G176" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
       <c r="I176" t="s">
-        <v>2889</v>
+        <v>2888</v>
       </c>
       <c r="W176">
         <v>1</v>
@@ -46611,10 +46605,10 @@
         <v>fauna</v>
       </c>
       <c r="F177" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G177" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="W177">
         <v>1</v>
@@ -47203,10 +47197,10 @@
         <v>gás</v>
       </c>
       <c r="F206" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="H206" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="M206">
         <v>1</v>
@@ -47229,13 +47223,13 @@
         <v>extra</v>
       </c>
       <c r="F207" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G207" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="H207" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
       <c r="AE207">
         <v>1</v>
@@ -47264,13 +47258,13 @@
         <v>extra</v>
       </c>
       <c r="F208" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="G208" t="s">
-        <v>2920</v>
+        <v>2919</v>
       </c>
       <c r="H208" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
       <c r="AE208">
         <v>1</v>
@@ -47299,13 +47293,13 @@
         <v>extra</v>
       </c>
       <c r="F209" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="G209" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="H209" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
       <c r="AE209">
         <v>1</v>

</xml_diff>

<commit_message>
conserta títulos / tira acentos de condition strings
</commit_message>
<xml_diff>
--- a/results/Perguntas.xlsx
+++ b/results/Perguntas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\Python\Filter-MSMARCO\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F09AF60-BEE8-47F6-99AE-F39B52D565FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67A7C3B-D35E-47F4-9A87-163AF1363657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17175" yWindow="-14730" windowWidth="11820" windowHeight="10335" tabRatio="566" firstSheet="2" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="566" firstSheet="2" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="filtered_qna_manual_sorted" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8927" uniqueCount="2930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8944" uniqueCount="2935">
   <si>
     <t>query</t>
   </si>
@@ -8169,9 +8169,6 @@
     <t>coral</t>
   </si>
   <si>
-    <t>tartaruga</t>
-  </si>
-  <si>
     <t>oceano</t>
   </si>
   <si>
@@ -8646,9 +8643,6 @@
     <t>marinho</t>
   </si>
   <si>
-    <t>polipo</t>
-  </si>
-  <si>
     <t>medusa</t>
   </si>
   <si>
@@ -8784,9 +8778,6 @@
     <t>As tartugas são animais aquáticos (vivem tanto em água doce quanto salgada), possuem o casco alto e achatado e as suas patas são em formato de remo, o que facilita seu deslocamento aquático. Há espécies carnívoras e outras herbívoras.</t>
   </si>
   <si>
-    <t>espécies</t>
-  </si>
-  <si>
     <t>diferença</t>
   </si>
   <si>
@@ -8811,9 +8802,6 @@
     <t>símbolo</t>
   </si>
   <si>
-    <t>energia_de_maré</t>
-  </si>
-  <si>
     <t>física</t>
   </si>
   <si>
@@ -8829,7 +8817,34 @@
     <t>prós</t>
   </si>
   <si>
-    <t>prós-contras</t>
+    <t>derramamento</t>
+  </si>
+  <si>
+    <t>plataforma</t>
+  </si>
+  <si>
+    <t>tartarugas</t>
+  </si>
+  <si>
+    <t>prós-e-contras</t>
+  </si>
+  <si>
+    <t>custo</t>
+  </si>
+  <si>
+    <t>extração</t>
+  </si>
+  <si>
+    <t>recurso-renovável</t>
+  </si>
+  <si>
+    <t>espécie</t>
+  </si>
+  <si>
+    <t>corais</t>
+  </si>
+  <si>
+    <t>pólipo</t>
   </si>
 </sst>
 </file>
@@ -42198,9 +42213,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17344D9D-8D84-42DD-9996-E6496156E107}">
   <dimension ref="A1:AF502"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G144" sqref="G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42231,85 +42246,85 @@
         <v>2572</v>
       </c>
       <c r="E1" t="s">
+        <v>2894</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2895</v>
+      </c>
+      <c r="G1" t="s">
         <v>2896</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>2897</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2898</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2899</v>
       </c>
       <c r="I1" t="s">
         <v>2573</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>2708</v>
+        <v>2933</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>2923</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>2912</v>
+        <v>2910</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>2927</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>2920</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>2709</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>2924</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>2710</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
+        <v>2899</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>2919</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>2711</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>2901</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>2922</v>
-      </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>2712</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>2713</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>2714</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>2715</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>2716</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>2717</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>2718</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>2719</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>2720</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>2721</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="6" t="s">
         <v>2722</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>2723</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
@@ -42318,20 +42333,17 @@
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D65" si="0">IF(AND(ISBLANK(F2),ISBLANK(G2),ISBLANK(H2)), E2, _xlfn.CONCAT(E2,"--",_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(ISBLANK(F2),"",_xlfn.CONCAT(F2,"-")),IF(ISBLANK(G2),"",_xlfn.CONCAT(G2,"-")),IF(ISBLANK(H2),"",_xlfn.CONCAT(H2,"-"))),IF(_xlpm.X="","",LEFT(_xlpm.X,LEN(_xlpm.X)-1)))))</f>
-        <v>coral-turismo--efeito-turismo-coral</v>
+        <v>corais-turismo--efeito-turismo</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" ref="E2:E30" si="1">_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(J2=1, _xlfn.CONCAT(J$1,"-"), ""), IF(K2=1, _xlfn.CONCAT(K$1,"-"), ""),IF(L2=1, _xlfn.CONCAT(L$1,"-"), ""),IF(M2=1, _xlfn.CONCAT(M$1,"-"), ""),IF(N2=1, _xlfn.CONCAT(N$1,"-"), ""),IF(O2=1, _xlfn.CONCAT(O$1,"-"), ""),IF(P2=1, _xlfn.CONCAT(P$1,"-"), ""),IF(Q2=1, _xlfn.CONCAT(Q$1,"-"), ""),IF(R2=1, _xlfn.CONCAT(R$1,"-"), ""),IF(S2=1, _xlfn.CONCAT(S$1,"-"), ""),IF(T2=1, _xlfn.CONCAT(T$1,"-"), ""),IF(U2=1, _xlfn.CONCAT(U$1,"-"), ""),IF(V2=1, _xlfn.CONCAT(V$1,"-"), ""),IF(W2=1, _xlfn.CONCAT(W$1,"-"), ""),IF(X2=1, _xlfn.CONCAT(X$1,"-"), ""),IF(Y2=1, _xlfn.CONCAT(Y$1,"-"), ""),IF(Z2=1, _xlfn.CONCAT(Z$1,"-"), ""),IF(AA2=1, _xlfn.CONCAT(AA$1,"-"), ""),IF(AB2=1, _xlfn.CONCAT(AB$1,"-"), ""),IF(AC2=1, _xlfn.CONCAT(AC$1,"-"), ""),IF(AD2=1, _xlfn.CONCAT(AD$1,"-"), ""),IF(AE2=1, _xlfn.CONCAT(AE$1,"-"), "")),LEFT(_xlpm.X,LEN(_xlpm.X)-1))</f>
-        <v>coral-turismo</v>
+        <v>corais-turismo</v>
       </c>
       <c r="F2" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="G2" t="s">
-        <v>2717</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2708</v>
+        <v>2716</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -42350,17 +42362,17 @@
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>coral--definir-recife</v>
+        <v>corais--definir-recife</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F3" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G3" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -42375,18 +42387,18 @@
         <v>2596</v>
       </c>
       <c r="B4" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>coral--definir</v>
+        <v>corais--definir</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F4" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -42401,18 +42413,18 @@
         <v>2597</v>
       </c>
       <c r="B5" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>coral--composição</v>
+        <v>corais--composição</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F5" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -42428,17 +42440,17 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>coral--definir-branqueamento</v>
+        <v>corais--definir-branqueamento</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F6" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G6" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -42454,17 +42466,17 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>coral--definir-recife</v>
+        <v>corais--definir-recife</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F7" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G7" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -42480,20 +42492,20 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>coral--listar-iniciativas-governo</v>
+        <v>corais--listar-iniciativas-governo</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F8" t="s">
+        <v>2842</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2850</v>
+      </c>
+      <c r="H8" t="s">
         <v>2843</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2851</v>
-      </c>
-      <c r="H8" t="s">
-        <v>2844</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -42509,17 +42521,17 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>coral--localização-recife</v>
+        <v>corais--localização-recife</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F9" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
       <c r="G9" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -42535,17 +42547,17 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>coral--listar-tipos</v>
+        <v>corais--listar-tipos</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F10" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="H10" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -42561,17 +42573,17 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>coral--definir-recife-artificial</v>
+        <v>corais--definir-recife-artificial</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F11" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G11" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -42587,20 +42599,20 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>coral--efeito-branqueamento-ambiente</v>
+        <v>corais--efeito-branqueamento-ambiente</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>coral</v>
+        <v>corais</v>
       </c>
       <c r="F12" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="G12" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="H12" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -42616,11 +42628,11 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>coral-símbolo</v>
+        <v>corais-símbolo</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>coral-símbolo</v>
+        <v>corais-símbolo</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -42639,20 +42651,17 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>energia_de_maré--efeito-energia-de-maré-ambiente</v>
+        <v>energia-de-maré--efeito-ambiente</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>energia_de_maré</v>
+        <v>energia-de-maré</v>
       </c>
       <c r="F14" t="s">
-        <v>2840</v>
-      </c>
-      <c r="G14" t="s">
-        <v>2927</v>
+        <v>2839</v>
       </c>
       <c r="H14" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -42668,20 +42677,20 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>energia_de_maré--efeito-energia-de-maré-economia</v>
+        <v>energia-de-maré--efeito-energia-de-maré-economia</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>energia_de_maré</v>
+        <v>energia-de-maré</v>
       </c>
       <c r="F15" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="G15" t="s">
-        <v>2927</v>
+        <v>2923</v>
       </c>
       <c r="H15" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -42693,21 +42702,21 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>energia_de_maré--listar-prós-contras</v>
+        <v>energia-de-maré--listar-prós-e-contras</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>energia_de_maré</v>
+        <v>energia-de-maré</v>
       </c>
       <c r="F16" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G16" t="s">
-        <v>2929</v>
+        <v>2928</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -42719,21 +42728,21 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2893</v>
+        <v>2891</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>energia_de_maré--listar-contras</v>
+        <v>energia-de-maré--listar-contras</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>energia_de_maré</v>
+        <v>energia-de-maré</v>
       </c>
       <c r="F17" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G17" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -42745,21 +42754,21 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>energia_de_maré--listar-prós</v>
+        <v>energia-de-maré--listar-prós</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>energia_de_maré</v>
+        <v>energia-de-maré</v>
       </c>
       <c r="F18" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G18" t="s">
-        <v>2928</v>
+        <v>2924</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -42775,14 +42784,14 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>energia_de_maré--localização</v>
+        <v>energia-de-maré--localização</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>energia_de_maré</v>
+        <v>energia-de-maré</v>
       </c>
       <c r="F19" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -42798,17 +42807,17 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>energia_de_maré--definir</v>
+        <v>energia-de-maré--definir</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>energia_de_maré</v>
+        <v>energia-de-maré</v>
       </c>
       <c r="F20" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="I20" t="s">
-        <v>2895</v>
+        <v>2893</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -42831,10 +42840,10 @@
         <v>petróleo</v>
       </c>
       <c r="F21" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="G21" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -42850,12 +42859,21 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>petróleo</v>
+        <v>petróleo--efeito-derramamento-ambiente</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
         <v>petróleo</v>
       </c>
+      <c r="F22" t="s">
+        <v>2839</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2925</v>
+      </c>
+      <c r="H22" t="s">
+        <v>2846</v>
+      </c>
       <c r="L22">
         <v>1</v>
       </c>
@@ -42870,12 +42888,21 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>petróleo</v>
+        <v>petróleo--efeito-derramamento-economia</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
         <v>petróleo</v>
       </c>
+      <c r="F23" t="s">
+        <v>2839</v>
+      </c>
+      <c r="G23" t="s">
+        <v>2925</v>
+      </c>
+      <c r="H23" t="s">
+        <v>2847</v>
+      </c>
       <c r="L23">
         <v>1</v>
       </c>
@@ -42890,12 +42917,18 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>petróleo</v>
+        <v>petróleo--definir-plataforma</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
         <v>petróleo</v>
       </c>
+      <c r="F24" t="s">
+        <v>2864</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2926</v>
+      </c>
       <c r="L24">
         <v>1</v>
       </c>
@@ -42906,16 +42939,22 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>petróleo</v>
+        <v>petróleo--quantidade-consumo</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
         <v>petróleo</v>
       </c>
+      <c r="F25" t="s">
+        <v>2855</v>
+      </c>
+      <c r="H25" t="s">
+        <v>2845</v>
+      </c>
       <c r="L25">
         <v>1</v>
       </c>
@@ -42930,12 +42969,21 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>petróleo</v>
+        <v>petróleo--definir-custo-extração</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
         <v>petróleo</v>
       </c>
+      <c r="F26" t="s">
+        <v>2864</v>
+      </c>
+      <c r="G26" t="s">
+        <v>2929</v>
+      </c>
+      <c r="H26" t="s">
+        <v>2930</v>
+      </c>
       <c r="L26">
         <v>1</v>
       </c>
@@ -42949,10 +42997,10 @@
         <v>2610</v>
       </c>
       <c r="B27" t="s">
+        <v>2745</v>
+      </c>
+      <c r="C27" t="s">
         <v>2746</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2747</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -42963,10 +43011,10 @@
         <v>petróleo</v>
       </c>
       <c r="F27" t="s">
+        <v>2852</v>
+      </c>
+      <c r="G27" t="s">
         <v>2853</v>
-      </c>
-      <c r="G27" t="s">
-        <v>2854</v>
       </c>
       <c r="L27">
         <v>1</v>
@@ -42978,7 +43026,7 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -42989,10 +43037,10 @@
         <v>petróleo</v>
       </c>
       <c r="F28" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="G28" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="L28">
         <v>1</v>
@@ -43004,13 +43052,13 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="C29" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="D29" t="str">
         <f>IF(AND(ISBLANK(F29),ISBLANK(G29),ISBLANK(H29)), E29, _xlfn.CONCAT(E29,"--",_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(ISBLANK(F29),"",_xlfn.CONCAT(F29,"-")),IF(ISBLANK(G29),"",_xlfn.CONCAT(G29,"-")),IF(ISBLANK(H29),"",_xlfn.CONCAT(H29,"-"))),IF(_xlpm.X="","",LEFT(_xlpm.X,LEN(_xlpm.X)-1)))))</f>
@@ -43021,13 +43069,13 @@
         <v>gás</v>
       </c>
       <c r="F29" t="s">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="G29" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="H29" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -43039,13 +43087,13 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
+        <v>2752</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>2753</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>2754</v>
-      </c>
       <c r="C30" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -43056,13 +43104,13 @@
         <v>petróleo</v>
       </c>
       <c r="F30" t="s">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="G30" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="H30" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="L30">
         <v>1</v>
@@ -43074,13 +43122,13 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>2748</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>2749</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>2750</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>2751</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -43091,7 +43139,7 @@
         <v>petróleo</v>
       </c>
       <c r="F31" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="L31">
         <v>1</v>
@@ -43103,10 +43151,10 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>2754</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>2755</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>2756</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -43117,10 +43165,10 @@
         <v>gás</v>
       </c>
       <c r="F32" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="H32" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -43136,12 +43184,18 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>petróleo</v>
+        <v>petróleo--definir-derramamento</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" ref="E33:E96" si="3">_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(J33=1, _xlfn.CONCAT(J$1,"-"), ""), IF(K33=1, _xlfn.CONCAT(K$1,"-"), ""),IF(L33=1, _xlfn.CONCAT(L$1,"-"), ""),IF(M33=1, _xlfn.CONCAT(M$1,"-"), ""),IF(N33=1, _xlfn.CONCAT(N$1,"-"), ""),IF(O33=1, _xlfn.CONCAT(O$1,"-"), ""),IF(P33=1, _xlfn.CONCAT(P$1,"-"), ""),IF(Q33=1, _xlfn.CONCAT(Q$1,"-"), ""),IF(R33=1, _xlfn.CONCAT(R$1,"-"), ""),IF(S33=1, _xlfn.CONCAT(S$1,"-"), ""),IF(T33=1, _xlfn.CONCAT(T$1,"-"), ""),IF(U33=1, _xlfn.CONCAT(U$1,"-"), ""),IF(V33=1, _xlfn.CONCAT(V$1,"-"), ""),IF(W33=1, _xlfn.CONCAT(W$1,"-"), ""),IF(X33=1, _xlfn.CONCAT(X$1,"-"), ""),IF(Y33=1, _xlfn.CONCAT(Y$1,"-"), ""),IF(Z33=1, _xlfn.CONCAT(Z$1,"-"), ""),IF(AA33=1, _xlfn.CONCAT(AA$1,"-"), ""),IF(AB33=1, _xlfn.CONCAT(AB$1,"-"), ""),IF(AC33=1, _xlfn.CONCAT(AC$1,"-"), ""),IF(AD33=1, _xlfn.CONCAT(AD$1,"-"), ""),IF(AE33=1, _xlfn.CONCAT(AE$1,"-"), "")),LEFT(_xlpm.X,LEN(_xlpm.X)-1))</f>
         <v>petróleo</v>
       </c>
+      <c r="F33" t="s">
+        <v>2864</v>
+      </c>
+      <c r="G33" t="s">
+        <v>2925</v>
+      </c>
       <c r="L33">
         <v>1</v>
       </c>
@@ -43156,12 +43210,18 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>petróleo</v>
+        <v>petróleo--maiores-derramamento</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="3"/>
         <v>petróleo</v>
       </c>
+      <c r="F34" t="s">
+        <v>2852</v>
+      </c>
+      <c r="G34" t="s">
+        <v>2925</v>
+      </c>
       <c r="L34">
         <v>1</v>
       </c>
@@ -43175,13 +43235,19 @@
         <v>2613</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>petróleo</v>
+        <f>IF(AND(ISBLANK(F35),ISBLANK(G35),ISBLANK(H35)), E35, _xlfn.CONCAT(E35,"--",_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(ISBLANK(F35),"",_xlfn.CONCAT(F35,"-")),IF(ISBLANK(G35),"",_xlfn.CONCAT(G35,"-")),IF(ISBLANK(H35),"",_xlfn.CONCAT(H35,"-"))),IF(_xlpm.X="","",LEFT(_xlpm.X,LEN(_xlpm.X)-1)))))</f>
+        <v>petróleo--pertence-recurso-renovável</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="3"/>
         <v>petróleo</v>
       </c>
+      <c r="F35" t="s">
+        <v>2860</v>
+      </c>
+      <c r="H35" t="s">
+        <v>2931</v>
+      </c>
       <c r="L35">
         <v>1</v>
       </c>
@@ -43258,7 +43324,7 @@
         <v>1559</v>
       </c>
       <c r="B39" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
@@ -43269,7 +43335,7 @@
         <v>petróleo</v>
       </c>
       <c r="F39" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -43404,13 +43470,13 @@
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
+        <v>2743</v>
+      </c>
+      <c r="B46" t="s">
         <v>2744</v>
       </c>
-      <c r="B46" t="s">
-        <v>2745</v>
-      </c>
       <c r="C46" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
@@ -43421,10 +43487,10 @@
         <v>petróleo</v>
       </c>
       <c r="F46" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="H46" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="L46">
         <v>1</v>
@@ -43439,24 +43505,24 @@
         <v>2574</v>
       </c>
       <c r="B47" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="C47" t="s">
         <v>2701</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--definir-dieta</v>
+        <v>tartarugas--definir-dieta</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F47" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="H47" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="N47">
         <v>1</v>
@@ -43472,11 +43538,11 @@
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga-símbolo</v>
+        <v>tartarugas-símbolo</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga-símbolo</v>
+        <v>tartarugas-símbolo</v>
       </c>
       <c r="N48">
         <v>1</v>
@@ -43494,21 +43560,21 @@
         <v>2576</v>
       </c>
       <c r="B49" t="s">
-        <v>2829</v>
+        <v>2828</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--listar-espécies</v>
+        <v>tartarugas--listar-espécie</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F49" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G49" t="s">
-        <v>2914</v>
+        <v>2932</v>
       </c>
       <c r="N49">
         <v>1</v>
@@ -43523,21 +43589,21 @@
         <v>2577</v>
       </c>
       <c r="B50" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--diferença-jabuti</v>
+        <v>tartarugas--diferença-jabuti</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F50" t="s">
-        <v>2915</v>
+        <v>2912</v>
       </c>
       <c r="G50" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="N50">
         <v>1</v>
@@ -43549,24 +43615,24 @@
     </row>
     <row r="51" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>2790</v>
+      </c>
+      <c r="B51" t="s">
         <v>2791</v>
-      </c>
-      <c r="B51" t="s">
-        <v>2792</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--pertence-jabuti</v>
+        <v>tartarugas--pertence-jabuti</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F51" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="G51" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -43578,24 +43644,24 @@
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>2792</v>
+      </c>
+      <c r="B52" t="s">
         <v>2793</v>
-      </c>
-      <c r="B52" t="s">
-        <v>2794</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--definir-quelônio</v>
+        <v>tartarugas--definir-quelônio</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F52" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G52" t="s">
-        <v>2925</v>
+        <v>2921</v>
       </c>
       <c r="N52">
         <v>1</v>
@@ -43610,21 +43676,21 @@
         <v>2578</v>
       </c>
       <c r="B53" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--definir-jabuti</v>
+        <v>tartarugas--definir-jabuti</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F53" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G53" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -43639,21 +43705,21 @@
         <v>2579</v>
       </c>
       <c r="B54" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--definir-cágado</v>
+        <v>tartarugas--definir-cágado</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F54" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G54" t="s">
-        <v>2926</v>
+        <v>2922</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -43668,18 +43734,18 @@
         <v>2580</v>
       </c>
       <c r="B55" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--definir</v>
+        <v>tartarugas--definir</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F55" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -43695,11 +43761,11 @@
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N56">
         <v>1</v>
@@ -43714,27 +43780,27 @@
         <v>2582</v>
       </c>
       <c r="B57" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="C57" t="s">
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--listar-espécies-extinção</v>
+        <v>tartarugas--listar-espécie-extinção</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F57" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G57" t="s">
-        <v>2914</v>
+        <v>2932</v>
       </c>
       <c r="H57" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="N57">
         <v>1</v>
@@ -43746,27 +43812,27 @@
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>2835</v>
+      </c>
+      <c r="B58" t="s">
         <v>2836</v>
-      </c>
-      <c r="B58" t="s">
-        <v>2837</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--motivo-extinção</v>
+        <v>tartarugas--motivo-extinção</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F58" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="H58" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="I58" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -43782,11 +43848,11 @@
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N59">
         <v>1</v>
@@ -43802,11 +43868,11 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N60">
         <v>1</v>
@@ -43822,11 +43888,11 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N61">
         <v>1</v>
@@ -43842,11 +43908,11 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N62">
         <v>1</v>
@@ -43861,21 +43927,21 @@
         <v>2587</v>
       </c>
       <c r="B63" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga--definir-ciclo-de-vida</v>
+        <v>tartarugas--definir-ciclo-de-vida</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F63" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G63" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="N63">
         <v>1</v>
@@ -43891,11 +43957,11 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N64">
         <v>1</v>
@@ -43911,11 +43977,11 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N65">
         <v>1</v>
@@ -43931,11 +43997,11 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" ref="D66:D129" si="4">IF(AND(ISBLANK(F66),ISBLANK(G66),ISBLANK(H66)), E66, _xlfn.CONCAT(E66,"--",_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(ISBLANK(F66),"",_xlfn.CONCAT(F66,"-")),IF(ISBLANK(G66),"",_xlfn.CONCAT(G66,"-")),IF(ISBLANK(H66),"",_xlfn.CONCAT(H66,"-"))),IF(_xlpm.X="","",LEFT(_xlpm.X,LEN(_xlpm.X)-1)))))</f>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N66">
         <v>1</v>
@@ -43950,18 +44016,18 @@
         <v>2591</v>
       </c>
       <c r="B67" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="4"/>
-        <v>tartaruga--localização</v>
+        <v>tartarugas--localização</v>
       </c>
       <c r="E67" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F67" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
       <c r="N67">
         <v>1</v>
@@ -43977,11 +44043,11 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="4"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N68">
         <v>1</v>
@@ -43997,11 +44063,11 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="4"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="N69">
         <v>1</v>
@@ -44023,17 +44089,17 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="4"/>
-        <v>tartaruga--definir-peso</v>
+        <v>tartarugas--definir-peso</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga</v>
+        <v>tartarugas</v>
       </c>
       <c r="F70" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G70" t="s">
-        <v>2858</v>
+        <v>2857</v>
       </c>
       <c r="N70">
         <v>1</v>
@@ -44049,11 +44115,11 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="4"/>
-        <v>tartaruga-corrente</v>
+        <v>tartarugas-corrente</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="3"/>
-        <v>tartaruga-corrente</v>
+        <v>tartarugas-corrente</v>
       </c>
       <c r="N71">
         <v>1</v>
@@ -44591,7 +44657,7 @@
     </row>
     <row r="98" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
-        <v>2903</v>
+        <v>2901</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="4"/>
@@ -44622,10 +44688,10 @@
         <v>oceano</v>
       </c>
       <c r="F99" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="G99" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="P99">
         <v>1</v>
@@ -44648,10 +44714,10 @@
         <v>extra</v>
       </c>
       <c r="F100" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G100" t="s">
-        <v>2902</v>
+        <v>2900</v>
       </c>
       <c r="AE100">
         <v>1</v>
@@ -44694,10 +44760,10 @@
         <v>oceano</v>
       </c>
       <c r="F102" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G102" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="P102">
         <v>1</v>
@@ -45106,7 +45172,7 @@
         <v>maré</v>
       </c>
       <c r="F122" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="R122">
         <v>1</v>
@@ -45129,10 +45195,10 @@
         <v>extra</v>
       </c>
       <c r="F123" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G123" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
       <c r="AE123">
         <v>1</v>
@@ -45473,10 +45539,10 @@
         <v>2706</v>
       </c>
       <c r="B140" t="s">
-        <v>2824</v>
+        <v>2823</v>
       </c>
       <c r="C140" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
       <c r="D140" t="str">
         <f t="shared" si="8"/>
@@ -45487,10 +45553,10 @@
         <v>flora</v>
       </c>
       <c r="F140" t="s">
+        <v>2864</v>
+      </c>
+      <c r="G140" t="s">
         <v>2865</v>
-      </c>
-      <c r="G140" t="s">
-        <v>2866</v>
       </c>
       <c r="V140">
         <v>1</v>
@@ -45502,13 +45568,13 @@
     </row>
     <row r="141" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
-        <v>2817</v>
+        <v>2816</v>
       </c>
       <c r="B141" t="s">
+        <v>2821</v>
+      </c>
+      <c r="C141" t="s">
         <v>2822</v>
-      </c>
-      <c r="C141" t="s">
-        <v>2823</v>
       </c>
       <c r="D141" t="str">
         <f t="shared" si="8"/>
@@ -45519,10 +45585,10 @@
         <v>flora-fauna</v>
       </c>
       <c r="F141" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G141" t="s">
-        <v>2921</v>
+        <v>2918</v>
       </c>
       <c r="V141">
         <v>1</v>
@@ -45537,13 +45603,13 @@
     </row>
     <row r="142" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
+        <v>2817</v>
+      </c>
+      <c r="B142" t="s">
+        <v>2819</v>
+      </c>
+      <c r="C142" t="s">
         <v>2818</v>
-      </c>
-      <c r="B142" t="s">
-        <v>2820</v>
-      </c>
-      <c r="C142" t="s">
-        <v>2819</v>
       </c>
       <c r="D142" t="str">
         <f t="shared" si="8"/>
@@ -45554,10 +45620,10 @@
         <v>flora-fauna</v>
       </c>
       <c r="F142" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G142" t="s">
-        <v>2920</v>
+        <v>2917</v>
       </c>
       <c r="V142">
         <v>1</v>
@@ -45572,27 +45638,27 @@
     </row>
     <row r="143" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A143" s="8" t="s">
+        <v>2777</v>
+      </c>
+      <c r="B143" t="s">
         <v>2778</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" t="s">
         <v>2779</v>
-      </c>
-      <c r="C143" t="s">
-        <v>2780</v>
       </c>
       <c r="D143" t="str">
         <f t="shared" si="8"/>
-        <v>fauna--definir-polipo</v>
+        <v>fauna--definir-pólipo</v>
       </c>
       <c r="E143" t="str">
         <f t="shared" si="6"/>
         <v>fauna</v>
       </c>
       <c r="F143" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G143" t="s">
-        <v>2868</v>
+        <v>2934</v>
       </c>
       <c r="W143">
         <v>1</v>
@@ -45604,13 +45670,13 @@
     </row>
     <row r="144" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A144" s="8" t="s">
+        <v>2768</v>
+      </c>
+      <c r="B144" t="s">
         <v>2769</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>2770</v>
-      </c>
-      <c r="C144" t="s">
-        <v>2771</v>
       </c>
       <c r="D144" t="str">
         <f t="shared" si="8"/>
@@ -45621,13 +45687,13 @@
         <v>fauna</v>
       </c>
       <c r="F144" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G144" t="s">
         <v>2708</v>
       </c>
       <c r="H144" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="W144">
         <v>1</v>
@@ -45639,10 +45705,10 @@
     </row>
     <row r="145" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A145" s="8" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="B145" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="D145" t="str">
         <f t="shared" si="8"/>
@@ -45653,10 +45719,10 @@
         <v>fauna</v>
       </c>
       <c r="F145" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G145" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
       <c r="W145">
         <v>1</v>
@@ -45668,10 +45734,10 @@
     </row>
     <row r="146" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A146" s="7" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="B146" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D146" t="str">
         <f t="shared" si="8"/>
@@ -45682,13 +45748,13 @@
         <v>fauna</v>
       </c>
       <c r="F146" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G146" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="H146" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="W146">
         <v>1</v>
@@ -45700,10 +45766,10 @@
     </row>
     <row r="147" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="B147" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="D147" t="str">
         <f t="shared" si="8"/>
@@ -45714,13 +45780,13 @@
         <v>fauna</v>
       </c>
       <c r="F147" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G147" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="H147" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="W147">
         <v>1</v>
@@ -45732,13 +45798,13 @@
     </row>
     <row r="148" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A148" s="7" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="B148" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="C148" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="D148" t="str">
         <f t="shared" si="8"/>
@@ -45749,10 +45815,10 @@
         <v>fauna</v>
       </c>
       <c r="F148" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G148" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="W148">
         <v>1</v>
@@ -45764,13 +45830,13 @@
     </row>
     <row r="149" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
+        <v>2800</v>
+      </c>
+      <c r="B149" t="s">
         <v>2801</v>
       </c>
-      <c r="B149" t="s">
-        <v>2802</v>
-      </c>
       <c r="C149" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="D149" t="str">
         <f t="shared" si="8"/>
@@ -45781,10 +45847,10 @@
         <v>fauna</v>
       </c>
       <c r="F149" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G149" t="s">
-        <v>2916</v>
+        <v>2913</v>
       </c>
       <c r="W149">
         <v>1</v>
@@ -45796,13 +45862,13 @@
     </row>
     <row r="150" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A150" s="7" t="s">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="B150" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="C150" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="D150" t="str">
         <f t="shared" si="8"/>
@@ -45813,10 +45879,10 @@
         <v>fauna</v>
       </c>
       <c r="F150" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G150" t="s">
-        <v>2917</v>
+        <v>2914</v>
       </c>
       <c r="W150">
         <v>1</v>
@@ -45828,7 +45894,7 @@
     </row>
     <row r="151" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
       <c r="D151" t="str">
         <f t="shared" si="8"/>
@@ -45839,13 +45905,13 @@
         <v>fauna</v>
       </c>
       <c r="F151" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="G151" t="s">
-        <v>2917</v>
+        <v>2914</v>
       </c>
       <c r="H151" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="W151">
         <v>1</v>
@@ -45860,10 +45926,10 @@
         <v>2679</v>
       </c>
       <c r="B152" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="C152" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="8"/>
@@ -45874,13 +45940,13 @@
         <v>fauna</v>
       </c>
       <c r="F152" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="G152" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="H152" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="W152">
         <v>1</v>
@@ -45892,10 +45958,10 @@
     </row>
     <row r="153" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="B153" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="D153" t="str">
         <f t="shared" si="8"/>
@@ -45906,10 +45972,10 @@
         <v>fauna</v>
       </c>
       <c r="F153" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
       <c r="G153" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="W153">
         <v>1</v>
@@ -45921,13 +45987,13 @@
     </row>
     <row r="154" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
+        <v>2813</v>
+      </c>
+      <c r="B154" t="s">
+        <v>2815</v>
+      </c>
+      <c r="C154" t="s">
         <v>2814</v>
-      </c>
-      <c r="B154" t="s">
-        <v>2816</v>
-      </c>
-      <c r="C154" t="s">
-        <v>2815</v>
       </c>
       <c r="D154" t="str">
         <f t="shared" si="8"/>
@@ -45938,10 +46004,10 @@
         <v>fauna-turismo</v>
       </c>
       <c r="F154" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
       <c r="G154" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="W154">
         <v>1</v>
@@ -46019,10 +46085,10 @@
         <v>2683</v>
       </c>
       <c r="B158" t="s">
-        <v>2831</v>
+        <v>2830</v>
       </c>
       <c r="C158" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
       <c r="D158" t="str">
         <f t="shared" si="8"/>
@@ -46033,10 +46099,10 @@
         <v>fauna</v>
       </c>
       <c r="F158" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G158" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
       <c r="W158">
         <v>1</v>
@@ -46048,13 +46114,13 @@
     </row>
     <row r="159" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A159" s="7" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
       <c r="B159" t="s">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="C159" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
       <c r="D159" t="str">
         <f t="shared" si="8"/>
@@ -46065,10 +46131,10 @@
         <v>fauna</v>
       </c>
       <c r="F159" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G159" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="W159">
         <v>1</v>
@@ -46080,10 +46146,10 @@
     </row>
     <row r="160" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A160" s="7" t="s">
+        <v>2775</v>
+      </c>
+      <c r="B160" t="s">
         <v>2776</v>
-      </c>
-      <c r="B160" t="s">
-        <v>2777</v>
       </c>
       <c r="D160" t="str">
         <f t="shared" si="8"/>
@@ -46094,10 +46160,10 @@
         <v>fauna</v>
       </c>
       <c r="F160" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G160" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="W160">
         <v>1</v>
@@ -46109,13 +46175,13 @@
     </row>
     <row r="161" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A161" s="7" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
       <c r="B161" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="C161" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
       <c r="D161" t="str">
         <f t="shared" si="8"/>
@@ -46126,10 +46192,10 @@
         <v>fauna</v>
       </c>
       <c r="F161" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G161" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="W161">
         <v>1</v>
@@ -46144,10 +46210,10 @@
         <v>2684</v>
       </c>
       <c r="B162" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
       <c r="C162" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
       <c r="D162" t="str">
         <f t="shared" si="8"/>
@@ -46158,10 +46224,10 @@
         <v>fauna</v>
       </c>
       <c r="F162" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G162" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="W162">
         <v>1</v>
@@ -46173,10 +46239,10 @@
     </row>
     <row r="163" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
+        <v>2784</v>
+      </c>
+      <c r="B163" t="s">
         <v>2785</v>
-      </c>
-      <c r="B163" t="s">
-        <v>2786</v>
       </c>
       <c r="D163" t="str">
         <f t="shared" si="8"/>
@@ -46187,10 +46253,10 @@
         <v>fauna</v>
       </c>
       <c r="F163" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G163" t="s">
-        <v>2872</v>
+        <v>2870</v>
       </c>
       <c r="W163">
         <v>1</v>
@@ -46205,10 +46271,10 @@
         <v>2685</v>
       </c>
       <c r="B164" t="s">
+        <v>2803</v>
+      </c>
+      <c r="C164" t="s">
         <v>2804</v>
-      </c>
-      <c r="C164" t="s">
-        <v>2805</v>
       </c>
       <c r="D164" t="str">
         <f t="shared" si="8"/>
@@ -46219,10 +46285,10 @@
         <v>fauna-turismo</v>
       </c>
       <c r="F164" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
       <c r="G164" t="s">
-        <v>2917</v>
+        <v>2914</v>
       </c>
       <c r="W164">
         <v>1</v>
@@ -46260,7 +46326,7 @@
         <v>2703</v>
       </c>
       <c r="B166" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
       <c r="D166" t="str">
         <f t="shared" si="8"/>
@@ -46271,10 +46337,10 @@
         <v>fauna</v>
       </c>
       <c r="F166" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G166" t="s">
-        <v>2918</v>
+        <v>2915</v>
       </c>
       <c r="W166">
         <v>1</v>
@@ -46289,10 +46355,10 @@
         <v>2704</v>
       </c>
       <c r="B167" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
       <c r="C167" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="D167" t="str">
         <f t="shared" si="8"/>
@@ -46303,10 +46369,10 @@
         <v>fauna</v>
       </c>
       <c r="F167" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G167" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
       <c r="W167">
         <v>1</v>
@@ -46321,7 +46387,7 @@
         <v>2705</v>
       </c>
       <c r="B168" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="D168" t="str">
         <f t="shared" si="8"/>
@@ -46332,10 +46398,10 @@
         <v>fauna</v>
       </c>
       <c r="F168" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G168" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
       <c r="W168">
         <v>1</v>
@@ -46350,7 +46416,7 @@
         <v>2707</v>
       </c>
       <c r="B169" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="D169" t="str">
         <f t="shared" si="8"/>
@@ -46361,10 +46427,10 @@
         <v>fauna</v>
       </c>
       <c r="F169" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G169" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
       <c r="W169">
         <v>1</v>
@@ -46376,7 +46442,7 @@
     </row>
     <row r="170" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
-        <v>2726</v>
+        <v>2725</v>
       </c>
       <c r="D170" t="str">
         <f t="shared" si="8"/>
@@ -46399,10 +46465,10 @@
         <v>2702</v>
       </c>
       <c r="B171" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
       <c r="C171" t="s">
-        <v>2743</v>
+        <v>2742</v>
       </c>
       <c r="D171" t="str">
         <f t="shared" si="8"/>
@@ -46413,10 +46479,10 @@
         <v>fauna</v>
       </c>
       <c r="F171" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G171" t="s">
-        <v>2918</v>
+        <v>2915</v>
       </c>
       <c r="W171">
         <v>1</v>
@@ -46428,10 +46494,10 @@
     </row>
     <row r="172" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A172" s="7" t="s">
+        <v>2730</v>
+      </c>
+      <c r="B172" t="s">
         <v>2731</v>
-      </c>
-      <c r="B172" t="s">
-        <v>2732</v>
       </c>
       <c r="D172" t="str">
         <f t="shared" si="8"/>
@@ -46442,10 +46508,10 @@
         <v>fauna</v>
       </c>
       <c r="F172" t="s">
-        <v>2884</v>
+        <v>2882</v>
       </c>
       <c r="G172" t="s">
-        <v>2918</v>
+        <v>2915</v>
       </c>
       <c r="W172">
         <v>1</v>
@@ -46457,13 +46523,13 @@
     </row>
     <row r="173" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
       <c r="B173" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="C173" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
       <c r="D173" t="str">
         <f t="shared" si="8"/>
@@ -46474,10 +46540,10 @@
         <v>fauna</v>
       </c>
       <c r="F173" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G173" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="W173">
         <v>1</v>
@@ -46489,13 +46555,13 @@
     </row>
     <row r="174" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
+        <v>2735</v>
+      </c>
+      <c r="B174" t="s">
         <v>2736</v>
       </c>
-      <c r="B174" t="s">
-        <v>2737</v>
-      </c>
       <c r="C174" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
       <c r="D174" t="str">
         <f t="shared" si="8"/>
@@ -46506,13 +46572,13 @@
         <v>fauna</v>
       </c>
       <c r="F174" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G174" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
       <c r="I174" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
       <c r="W174">
         <v>1</v>
@@ -46524,13 +46590,13 @@
     </row>
     <row r="175" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
       <c r="B175" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="C175" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
       <c r="D175" t="str">
         <f t="shared" si="8"/>
@@ -46541,10 +46607,10 @@
         <v>fauna</v>
       </c>
       <c r="F175" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G175" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="W175">
         <v>1</v>
@@ -46556,13 +46622,13 @@
     </row>
     <row r="176" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A176" s="7" t="s">
+        <v>2762</v>
+      </c>
+      <c r="B176" t="s">
+        <v>2887</v>
+      </c>
+      <c r="C176" t="s">
         <v>2763</v>
-      </c>
-      <c r="B176" t="s">
-        <v>2889</v>
-      </c>
-      <c r="C176" t="s">
-        <v>2764</v>
       </c>
       <c r="D176" t="str">
         <f t="shared" si="8"/>
@@ -46573,13 +46639,13 @@
         <v>fauna</v>
       </c>
       <c r="F176" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="G176" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
       <c r="I176" t="s">
-        <v>2888</v>
+        <v>2886</v>
       </c>
       <c r="W176">
         <v>1</v>
@@ -46591,10 +46657,10 @@
     </row>
     <row r="177" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A177" s="7" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="B177" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="D177" t="str">
         <f t="shared" si="8"/>
@@ -46605,10 +46671,10 @@
         <v>fauna</v>
       </c>
       <c r="F177" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G177" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="W177">
         <v>1</v>
@@ -46660,7 +46726,7 @@
     </row>
     <row r="180" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A180" s="7" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="D180" t="str">
         <f t="shared" si="8"/>
@@ -47183,10 +47249,10 @@
         <v>2642</v>
       </c>
       <c r="B206" t="s">
-        <v>2757</v>
+        <v>2756</v>
       </c>
       <c r="C206" s="10" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="D206" t="str">
         <f t="shared" si="10"/>
@@ -47197,10 +47263,10 @@
         <v>gás</v>
       </c>
       <c r="F206" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="H206" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="M206">
         <v>1</v>
@@ -47223,13 +47289,13 @@
         <v>extra</v>
       </c>
       <c r="F207" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="G207" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
       <c r="H207" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
       <c r="AE207">
         <v>1</v>
@@ -47241,13 +47307,13 @@
     </row>
     <row r="208" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
       <c r="B208" t="s">
+        <v>2727</v>
+      </c>
+      <c r="C208" t="s">
         <v>2728</v>
-      </c>
-      <c r="C208" t="s">
-        <v>2729</v>
       </c>
       <c r="D208" t="str">
         <f t="shared" si="10"/>
@@ -47258,13 +47324,13 @@
         <v>extra</v>
       </c>
       <c r="F208" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="G208" t="s">
-        <v>2919</v>
+        <v>2916</v>
       </c>
       <c r="H208" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
       <c r="AE208">
         <v>1</v>
@@ -47276,13 +47342,13 @@
     </row>
     <row r="209" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
       <c r="B209" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
       <c r="C209" t="s">
-        <v>2727</v>
+        <v>2726</v>
       </c>
       <c r="D209" t="str">
         <f t="shared" si="10"/>
@@ -47293,13 +47359,13 @@
         <v>extra</v>
       </c>
       <c r="F209" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="G209" t="s">
-        <v>2864</v>
+        <v>2863</v>
       </c>
       <c r="H209" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
       <c r="AE209">
         <v>1</v>

</xml_diff>

<commit_message>
mais perguntas e respostas
</commit_message>
<xml_diff>
--- a/results/Perguntas.xlsx
+++ b/results/Perguntas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\Python\Filter-MSMARCO\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB57494B-2FE6-495F-900E-4F0534985F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441517B5-8BE1-43BD-95B6-F99ED389E55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="60" windowWidth="14784" windowHeight="11964" tabRatio="565" firstSheet="2" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" tabRatio="565" firstSheet="3" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="filtered_qna_manual_sorted" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9073" uniqueCount="3000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9097" uniqueCount="3017">
   <si>
     <t>query</t>
   </si>
@@ -8457,9 +8457,6 @@
     <t>Peixes são animais aquáticos que possuem crânio, brânquias (guelras) e membros transformados em barbatanas ou nadadeiras. Essa definição inclui muitos seres vivos. Normalmente, quando falamos de peixes estamos nos referindo aos actinoperígeos, grupo ao qual pertencem cerca de 99% dos peixes vivos hoje.</t>
   </si>
   <si>
-    <t>Tubarões são peixes de esqueleto cartilaginoso, corpo hidrodinâmico (salvo exceções), com 5 a 7 fendas branquiais, que geralmente vivem em água salgada. Eles são conhecidos por serem exímios caçadores, capazes de farejar e detectar presas através de impulsos elétricos.</t>
-  </si>
-  <si>
     <t>Considerando o volume ocupado, a baleia-azul ganha de longe a competição, alcançando até 35 metros de comprimento e 160 toneladas de peso. Ela habita a maioria dos oceanos do planeta, sendo raras vezes avistada no Brasil, longe da costa.</t>
   </si>
   <si>
@@ -9040,6 +9037,60 @@
   </si>
   <si>
     <t>Impactos ambientais da energia de maré?</t>
+  </si>
+  <si>
+    <t>Tubarões são peixes de esqueleto cartilaginoso, corpo hidrodinâmico, com 5 a 7 fendas branquiais e que geralmente vivem em água salgada. Eles são conhecidos por serem exímios caçadores, capazes de farejar presas a longas distâncias e detectá-las através de impulsos elétricos.</t>
+  </si>
+  <si>
+    <t>Sim! Tubarões são um tipo de peixe.</t>
+  </si>
+  <si>
+    <t>frequência</t>
+  </si>
+  <si>
+    <t>Isso depende do local. No regime mais comum, o semi-diurno, a média é de 12 horas e 24 minutos.</t>
+  </si>
+  <si>
+    <t>Depende do local, mas o mais comum é 2 ciclos completos por dia (a maré enche e esvazia duas vezes).</t>
+  </si>
+  <si>
+    <t>A diferença do nível do mar entre as marés, conhecido como a amplitude da maré, varia muito de local a local. Em um mesmo local, também é possível que a primeira alta do dia seja maior que a segunda alta, por exemplo.</t>
+  </si>
+  <si>
+    <t>https://pt.wikipedia.org/wiki/Mar%C3%A9#Caracter%C3%ADsticas</t>
+  </si>
+  <si>
+    <t>O mais comum é um regime semi-diurno, em que ocorrem 2 ciclos de maré ao longo do dia (ou seja, a maré sobe e desce duas vezes no dia). O segundo tipo mais comum é o diurno, em que o ciclo ocorre uma vez ao dia. O terceiro tipo, chamado de misto, é bem menos comum e apresenta um ou dois ciclos por dia, mas com grande diferença de altura entre uma maré alta e outra, assim como entre as baixas.</t>
+  </si>
+  <si>
+    <t>Qual é a periodicidade das marés?--Quais são os regimes de marés?</t>
+  </si>
+  <si>
+    <t>Um dia de maré é o tempo que normalmente passa entre duas marés altas em um regime semi-diurno. Ele vale, na média, 24 horas e 51 minutos.</t>
+  </si>
+  <si>
+    <t>A maré é controlada, principalmente, pela atração gravitacional da Lua e do Sol.</t>
+  </si>
+  <si>
+    <t>As marés são causadas pelo efeito combinado das forças gravitacionais exercidas pela Lua e pelo Sol na terra.</t>
+  </si>
+  <si>
+    <t>Correntes oceânicas são o movimento contínuo, previsível e direcional de água nos oceanos.</t>
+  </si>
+  <si>
+    <t>O que causa as correntes oceânicas?</t>
+  </si>
+  <si>
+    <t>Isso depende, principalmente, do tamanho da tartaruga adulta de cada espécie. Para as tartarugas bem pequenas (menos que 10 cm de comprimento), pode ser 2 a 3 anos, enquanto as maiores podem levar até 50 anos para atingir a maturidade sexual.</t>
+  </si>
+  <si>
+    <t>https://www.britannica.com/animal/turtle-reptile/Reproduction#:~:text=The%20age%20at%20which%20turtles,and%20become%20sexually%20mature%20at</t>
+  </si>
+  <si>
+    <t>Assim como muitas outras espécies do reino animal, as tartarugas acasalam em um ritual que envolve o macho montar nas costas da fêmea. Devido à posição da cauda, que atrapalha, é necessária a cooperação da fêmea, que os machos obtêm através de mordidas e comportamento agressivo até a submissão, ou através de excitação, vibrando as patas dianteiras nos ombros e cabeça da fêmea.</t>
+  </si>
+  <si>
+    <t>https://www.britannica.com/animal/turtle-reptile/Reproduction</t>
   </si>
 </sst>
 </file>
@@ -42427,8 +42478,8 @@
   <dimension ref="A1:AE503"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42459,37 +42510,37 @@
         <v>2572</v>
       </c>
       <c r="E1" t="s">
+        <v>2886</v>
+      </c>
+      <c r="F1" t="s">
         <v>2887</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2888</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2889</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2890</v>
       </c>
       <c r="I1" t="s">
         <v>2573</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>2958</v>
+        <v>2957</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>2901</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>2902</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>2903</v>
-      </c>
       <c r="N1" s="4" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>2708</v>
@@ -42498,7 +42549,7 @@
         <v>2709</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>2710</v>
@@ -42528,13 +42579,13 @@
         <v>2718</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>2954</v>
+        <v>2953</v>
       </c>
       <c r="AC1" s="4" t="s">
         <v>2719</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
@@ -42542,10 +42593,10 @@
         <v>2594</v>
       </c>
       <c r="B2" t="s">
+        <v>2967</v>
+      </c>
+      <c r="C2" t="s">
         <v>2968</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2969</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D69" si="0">IF(AND(ISBLANK(F2),ISBLANK(G2),ISBLANK(H2)), E2, _xlfn.CONCAT(E2,"--",_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(ISBLANK(F2),"",_xlfn.CONCAT(F2,"-")),IF(ISBLANK(G2),"",_xlfn.CONCAT(G2,"-")),IF(ISBLANK(H2),"",_xlfn.CONCAT(H2,"-"))),IF(_xlpm.X="","",LEFT(_xlpm.X,LEN(_xlpm.X)-1)))))</f>
@@ -42556,7 +42607,7 @@
         <v>coral-turismo</v>
       </c>
       <c r="F2" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="G2" t="s">
         <v>2715</v>
@@ -42577,10 +42628,10 @@
         <v>2595</v>
       </c>
       <c r="B3" t="s">
+        <v>2969</v>
+      </c>
+      <c r="C3" t="s">
         <v>2970</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2971</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
@@ -42591,10 +42642,10 @@
         <v>coral</v>
       </c>
       <c r="F3" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G3" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -42620,7 +42671,7 @@
         <v>coral</v>
       </c>
       <c r="F4" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -42646,7 +42697,7 @@
         <v>coral</v>
       </c>
       <c r="F5" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -42661,7 +42712,7 @@
         <v>2598</v>
       </c>
       <c r="B6" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -42672,10 +42723,10 @@
         <v>coral</v>
       </c>
       <c r="F6" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G6" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -42687,10 +42738,10 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>2965</v>
+      </c>
+      <c r="B7" t="s">
         <v>2966</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2967</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ref="D7:D8" si="3">IF(AND(ISBLANK(F7),ISBLANK(G7),ISBLANK(H7)), E7, _xlfn.CONCAT(E7,"--",_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(ISBLANK(F7),"",_xlfn.CONCAT(F7,"-")),IF(ISBLANK(G7),"",_xlfn.CONCAT(G7,"-")),IF(ISBLANK(H7),"",_xlfn.CONCAT(H7,"-"))),IF(_xlpm.X="","",LEFT(_xlpm.X,LEN(_xlpm.X)-1)))))</f>
@@ -42701,10 +42752,10 @@
         <v>coral</v>
       </c>
       <c r="F7" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="G7" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -42719,10 +42770,10 @@
         <v>2599</v>
       </c>
       <c r="B8" t="s">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="C8" t="s">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="3"/>
@@ -42733,13 +42784,13 @@
         <v>coral</v>
       </c>
       <c r="F8" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="G8" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="H8" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -42751,13 +42802,13 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>2973</v>
+      </c>
+      <c r="B9" t="s">
         <v>2974</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>2975</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2976</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -42768,13 +42819,13 @@
         <v>coral</v>
       </c>
       <c r="F9" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="G9" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="H9" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -42797,13 +42848,13 @@
         <v>coral</v>
       </c>
       <c r="F10" t="s">
+        <v>2837</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2845</v>
+      </c>
+      <c r="H10" t="s">
         <v>2838</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2846</v>
-      </c>
-      <c r="H10" t="s">
-        <v>2839</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -42818,10 +42869,10 @@
         <v>2601</v>
       </c>
       <c r="B11" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="C11" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -42832,10 +42883,10 @@
         <v>coral</v>
       </c>
       <c r="F11" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="G11" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -42850,10 +42901,10 @@
         <v>2602</v>
       </c>
       <c r="B12" t="s">
-        <v>2977</v>
+        <v>2976</v>
       </c>
       <c r="C12" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -42864,10 +42915,10 @@
         <v>coral</v>
       </c>
       <c r="F12" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="H12" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -42882,10 +42933,10 @@
         <v>2603</v>
       </c>
       <c r="B13" t="s">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="C13" t="s">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -42896,10 +42947,10 @@
         <v>coral</v>
       </c>
       <c r="F13" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G13" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -42914,7 +42965,7 @@
         <v>2604</v>
       </c>
       <c r="B14" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -42925,13 +42976,13 @@
         <v>coral</v>
       </c>
       <c r="F14" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="G14" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="H14" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -42943,10 +42994,10 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="B15" t="s">
-        <v>2984</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
@@ -42954,10 +43005,10 @@
         <v>1027</v>
       </c>
       <c r="B16" t="s">
+        <v>2984</v>
+      </c>
+      <c r="C16" t="s">
         <v>2985</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2986</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -42968,10 +43019,10 @@
         <v>coral</v>
       </c>
       <c r="F16" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H16" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -42983,10 +43034,10 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2999</v>
+        <v>2998</v>
       </c>
       <c r="B17" t="s">
-        <v>2995</v>
+        <v>2994</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -42997,10 +43048,10 @@
         <v>energia-de-maré</v>
       </c>
       <c r="F17" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="H17" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -43012,13 +43063,13 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
       <c r="B18" t="s">
-        <v>2997</v>
+        <v>2996</v>
       </c>
       <c r="C18" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -43029,10 +43080,10 @@
         <v>energia-de-maré</v>
       </c>
       <c r="F18" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G18" t="s">
-        <v>2920</v>
+        <v>2919</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -43044,13 +43095,13 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>2885</v>
+        <v>2884</v>
       </c>
       <c r="B19" t="s">
-        <v>2998</v>
+        <v>2997</v>
       </c>
       <c r="C19" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -43061,10 +43112,10 @@
         <v>energia-de-maré</v>
       </c>
       <c r="F19" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G19" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -43076,13 +43127,13 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="B20" t="s">
-        <v>2996</v>
+        <v>2995</v>
       </c>
       <c r="C20" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -43093,10 +43144,10 @@
         <v>energia-de-maré</v>
       </c>
       <c r="F20" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G20" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -43111,10 +43162,10 @@
         <v>2605</v>
       </c>
       <c r="B21" t="s">
-        <v>2994</v>
+        <v>2993</v>
       </c>
       <c r="C21" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -43125,7 +43176,7 @@
         <v>energia-de-maré</v>
       </c>
       <c r="F21" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -43137,13 +43188,13 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>2990</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2992</v>
+      </c>
+      <c r="C22" t="s">
         <v>2991</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2993</v>
-      </c>
-      <c r="C22" t="s">
-        <v>2992</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" ref="D22:D23" si="6">IF(AND(ISBLANK(F22),ISBLANK(G22),ISBLANK(H22)), E22, _xlfn.CONCAT(E22,"--",_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(ISBLANK(F22),"",_xlfn.CONCAT(F22,"-")),IF(ISBLANK(G22),"",_xlfn.CONCAT(G22,"-")),IF(ISBLANK(H22),"",_xlfn.CONCAT(H22,"-"))),IF(_xlpm.X="","",LEFT(_xlpm.X,LEN(_xlpm.X)-1)))))</f>
@@ -43154,10 +43205,10 @@
         <v>energia-de-maré</v>
       </c>
       <c r="F22" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="G22" t="s">
-        <v>2988</v>
+        <v>2987</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -43169,13 +43220,13 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
       <c r="B23" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="C23" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="6"/>
@@ -43186,7 +43237,7 @@
         <v>energia-de-maré</v>
       </c>
       <c r="F23" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -43209,13 +43260,13 @@
         <v>oceano</v>
       </c>
       <c r="F24" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G24" t="s">
-        <v>2989</v>
+        <v>2988</v>
       </c>
       <c r="H24" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="P24">
         <v>1</v>
@@ -43238,10 +43289,10 @@
         <v>petróleo</v>
       </c>
       <c r="F25" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="G25" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="L25">
         <v>1</v>
@@ -43264,13 +43315,13 @@
         <v>petróleo</v>
       </c>
       <c r="F26" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="G26" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="H26" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -43293,13 +43344,13 @@
         <v>petróleo</v>
       </c>
       <c r="F27" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="G27" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="H27" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="L27">
         <v>1</v>
@@ -43322,10 +43373,10 @@
         <v>petróleo</v>
       </c>
       <c r="F28" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G28" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="L28">
         <v>1</v>
@@ -43348,10 +43399,10 @@
         <v>petróleo</v>
       </c>
       <c r="F29" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="H29" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="L29">
         <v>1</v>
@@ -43374,13 +43425,13 @@
         <v>petróleo</v>
       </c>
       <c r="F30" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="G30" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="H30" t="s">
-        <v>2921</v>
+        <v>2920</v>
       </c>
       <c r="L30">
         <v>1</v>
@@ -43409,10 +43460,10 @@
         <v>petróleo</v>
       </c>
       <c r="F31" t="s">
+        <v>2847</v>
+      </c>
+      <c r="G31" t="s">
         <v>2848</v>
-      </c>
-      <c r="G31" t="s">
-        <v>2849</v>
       </c>
       <c r="L31">
         <v>1</v>
@@ -43424,7 +43475,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -43435,10 +43486,10 @@
         <v>petróleo</v>
       </c>
       <c r="F32" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="G32" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -43467,13 +43518,13 @@
         <v>gás</v>
       </c>
       <c r="F33" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="G33" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="H33" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="M33">
         <v>1</v>
@@ -43502,13 +43553,13 @@
         <v>petróleo</v>
       </c>
       <c r="F34" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="G34" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="H34" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="L34">
         <v>1</v>
@@ -43537,7 +43588,7 @@
         <v>petróleo</v>
       </c>
       <c r="F35" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="L35">
         <v>1</v>
@@ -43563,10 +43614,10 @@
         <v>gás</v>
       </c>
       <c r="F36" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H36" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="M36">
         <v>1</v>
@@ -43589,10 +43640,10 @@
         <v>petróleo</v>
       </c>
       <c r="F37" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G37" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="L37">
         <v>1</v>
@@ -43615,10 +43666,10 @@
         <v>petróleo</v>
       </c>
       <c r="F38" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="G38" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="L38">
         <v>1</v>
@@ -43641,10 +43692,10 @@
         <v>petróleo</v>
       </c>
       <c r="F39" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="H39" t="s">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -43667,10 +43718,10 @@
         <v>petróleo</v>
       </c>
       <c r="F40" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H40" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
       <c r="L40">
         <v>1</v>
@@ -43693,13 +43744,13 @@
         <v>petróleo</v>
       </c>
       <c r="F41" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G41" t="s">
+        <v>2928</v>
+      </c>
+      <c r="H41" t="s">
         <v>2929</v>
-      </c>
-      <c r="H41" t="s">
-        <v>2930</v>
       </c>
       <c r="L41">
         <v>1</v>
@@ -43722,10 +43773,10 @@
         <v>petróleo-gás</v>
       </c>
       <c r="F42" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="G42" t="s">
-        <v>2933</v>
+        <v>2932</v>
       </c>
       <c r="L42">
         <v>1</v>
@@ -43754,7 +43805,7 @@
         <v>petróleo</v>
       </c>
       <c r="F43" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="L43">
         <v>1</v>
@@ -43777,13 +43828,13 @@
         <v>petróleo</v>
       </c>
       <c r="F44" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G44" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="H44" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
       <c r="L44">
         <v>1</v>
@@ -43806,10 +43857,10 @@
         <v>petróleo-engenharia</v>
       </c>
       <c r="F45" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="G45" t="s">
-        <v>2931</v>
+        <v>2930</v>
       </c>
       <c r="L45">
         <v>1</v>
@@ -43835,10 +43886,10 @@
         <v>petróleo</v>
       </c>
       <c r="F46" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="G46" t="s">
-        <v>2932</v>
+        <v>2931</v>
       </c>
       <c r="L46">
         <v>1</v>
@@ -43861,7 +43912,7 @@
         <v>petróleo</v>
       </c>
       <c r="F47" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="L47">
         <v>1</v>
@@ -43884,7 +43935,7 @@
         <v>petróleo</v>
       </c>
       <c r="F48" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="L48">
         <v>1</v>
@@ -43907,10 +43958,10 @@
         <v>petróleo</v>
       </c>
       <c r="F49" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G49" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
       <c r="L49">
         <v>1</v>
@@ -43939,10 +43990,10 @@
         <v>petróleo</v>
       </c>
       <c r="F50" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H50" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="L50">
         <v>1</v>
@@ -43971,10 +44022,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F51" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H51" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -43997,10 +44048,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F52" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H52" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="N52">
         <v>1</v>
@@ -44015,7 +44066,7 @@
         <v>2576</v>
       </c>
       <c r="B53" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
@@ -44026,10 +44077,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F53" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G53" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -44044,7 +44095,7 @@
         <v>2577</v>
       </c>
       <c r="B54" t="s">
-        <v>2823</v>
+        <v>2822</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
@@ -44055,13 +44106,13 @@
         <v>tartarugas</v>
       </c>
       <c r="F54" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="G54" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="H54" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -44087,13 +44138,13 @@
         <v>tartarugas</v>
       </c>
       <c r="F55" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="G55" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="H55" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -44119,10 +44170,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F56" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G56" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="N56">
         <v>1</v>
@@ -44137,7 +44188,7 @@
         <v>2578</v>
       </c>
       <c r="B57" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
@@ -44148,10 +44199,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F57" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G57" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="N57">
         <v>1</v>
@@ -44166,7 +44217,7 @@
         <v>2579</v>
       </c>
       <c r="B58" t="s">
-        <v>2822</v>
+        <v>2821</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
@@ -44177,10 +44228,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F58" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G58" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -44195,7 +44246,7 @@
         <v>2580</v>
       </c>
       <c r="B59" t="s">
-        <v>2963</v>
+        <v>2962</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
@@ -44206,7 +44257,7 @@
         <v>tartarugas</v>
       </c>
       <c r="F59" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="N59">
         <v>1</v>
@@ -44229,10 +44280,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F60" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="G60" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="N60">
         <v>1</v>
@@ -44247,10 +44298,10 @@
         <v>2582</v>
       </c>
       <c r="B61" t="s">
-        <v>2964</v>
+        <v>2963</v>
       </c>
       <c r="C61" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
@@ -44261,13 +44312,13 @@
         <v>tartarugas</v>
       </c>
       <c r="F61" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G61" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="H61" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="N61">
         <v>1</v>
@@ -44279,10 +44330,10 @@
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>2830</v>
+      </c>
+      <c r="B62" t="s">
         <v>2831</v>
-      </c>
-      <c r="B62" t="s">
-        <v>2832</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
@@ -44293,13 +44344,13 @@
         <v>tartarugas</v>
       </c>
       <c r="F62" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="H62" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="I62" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="N62">
         <v>1</v>
@@ -44322,10 +44373,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F63" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H63" t="s">
-        <v>2927</v>
+        <v>2926</v>
       </c>
       <c r="N63">
         <v>1</v>
@@ -44348,10 +44399,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F64" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G64" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="N64">
         <v>1</v>
@@ -44365,6 +44416,12 @@
       <c r="A65" t="s">
         <v>2585</v>
       </c>
+      <c r="B65" t="s">
+        <v>3015</v>
+      </c>
+      <c r="C65" t="s">
+        <v>3016</v>
+      </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
         <v>tartarugas--detalhar-reprodução</v>
@@ -44374,10 +44431,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F65" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H65" t="s">
-        <v>2940</v>
+        <v>2939</v>
       </c>
       <c r="N65">
         <v>1</v>
@@ -44400,10 +44457,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F66" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="H66" t="s">
-        <v>2942</v>
+        <v>2941</v>
       </c>
       <c r="N66">
         <v>1</v>
@@ -44418,7 +44475,7 @@
         <v>2587</v>
       </c>
       <c r="B67" t="s">
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
@@ -44429,10 +44486,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F67" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="H67" t="s">
-        <v>2858</v>
+        <v>2857</v>
       </c>
       <c r="N67">
         <v>1</v>
@@ -44455,10 +44512,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F68" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H68" t="s">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="N68">
         <v>1</v>
@@ -44481,10 +44538,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F69" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H69" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="N69">
         <v>1</v>
@@ -44507,10 +44564,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F70" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H70" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
       <c r="N70">
         <v>1</v>
@@ -44525,7 +44582,7 @@
         <v>2591</v>
       </c>
       <c r="B71" t="s">
-        <v>2824</v>
+        <v>2823</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="8"/>
@@ -44536,7 +44593,7 @@
         <v>tartarugas</v>
       </c>
       <c r="F71" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="N71">
         <v>1</v>
@@ -44550,6 +44607,12 @@
       <c r="A72" t="s">
         <v>2592</v>
       </c>
+      <c r="B72" t="s">
+        <v>3013</v>
+      </c>
+      <c r="C72" t="s">
+        <v>3014</v>
+      </c>
       <c r="D72" t="str">
         <f t="shared" si="8"/>
         <v>tartarugas--detalhar-idade-reprodutiva</v>
@@ -44559,10 +44622,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F72" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H72" t="s">
-        <v>2947</v>
+        <v>2946</v>
       </c>
       <c r="N72">
         <v>1</v>
@@ -44585,10 +44648,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F73" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H73" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
       <c r="N73">
         <v>1</v>
@@ -44617,10 +44680,10 @@
         <v>tartarugas</v>
       </c>
       <c r="F74" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H74" t="s">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="N74">
         <v>1</v>
@@ -44643,10 +44706,10 @@
         <v>corrente</v>
       </c>
       <c r="F75" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="H75" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="S75">
         <v>1</v>
@@ -44669,10 +44732,10 @@
         <v>oceano</v>
       </c>
       <c r="F76" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="G76" t="s">
-        <v>2948</v>
+        <v>2947</v>
       </c>
       <c r="P76">
         <v>1</v>
@@ -44695,10 +44758,10 @@
         <v>oceano</v>
       </c>
       <c r="F77" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H77" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="P77">
         <v>1</v>
@@ -44721,10 +44784,10 @@
         <v>oceano</v>
       </c>
       <c r="F78" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="G78" t="s">
-        <v>2953</v>
+        <v>2952</v>
       </c>
       <c r="P78">
         <v>1</v>
@@ -44747,10 +44810,10 @@
         <v>oceano</v>
       </c>
       <c r="F79" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="H79" t="s">
-        <v>2952</v>
+        <v>2951</v>
       </c>
       <c r="P79">
         <v>1</v>
@@ -44773,10 +44836,10 @@
         <v>petróleo</v>
       </c>
       <c r="F80" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H80" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="L80">
         <v>1</v>
@@ -44799,10 +44862,10 @@
         <v>oceano</v>
       </c>
       <c r="F81" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="H81" t="s">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="P81">
         <v>1</v>
@@ -44825,10 +44888,10 @@
         <v>oceano</v>
       </c>
       <c r="F82" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="G82" t="s">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="P82">
         <v>1</v>
@@ -44851,10 +44914,10 @@
         <v>oceano</v>
       </c>
       <c r="F83" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="G83" t="s">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="I83" t="s">
         <v>1431</v>
@@ -44880,10 +44943,10 @@
         <v>oceano</v>
       </c>
       <c r="F84" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H84" t="s">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="I84" s="7" t="s">
         <v>1446</v>
@@ -44909,13 +44972,13 @@
         <v>oceano</v>
       </c>
       <c r="F85" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="G85" t="s">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="H85" t="s">
-        <v>2952</v>
+        <v>2951</v>
       </c>
       <c r="P85">
         <v>1</v>
@@ -44938,10 +45001,10 @@
         <v>oceano</v>
       </c>
       <c r="F86" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="G86" t="s">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="H86" t="s">
         <v>2708</v>
@@ -44967,7 +45030,7 @@
         <v>oceano</v>
       </c>
       <c r="F87" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="P87">
         <v>1</v>
@@ -44990,10 +45053,10 @@
         <v>oceano</v>
       </c>
       <c r="F88" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G88" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="I88" s="7" t="s">
         <v>1325</v>
@@ -45008,7 +45071,7 @@
     </row>
     <row r="89" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
-        <v>2949</v>
+        <v>2948</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="8"/>
@@ -45019,10 +45082,10 @@
         <v>petróleo</v>
       </c>
       <c r="F89" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="H89" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="L89">
         <v>1</v>
@@ -45045,10 +45108,10 @@
         <v>oceano</v>
       </c>
       <c r="F90" t="s">
-        <v>2955</v>
+        <v>2954</v>
       </c>
       <c r="G90" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="P90">
         <v>1</v>
@@ -45060,7 +45123,7 @@
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
-        <v>2956</v>
+        <v>2955</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" ref="D91" si="11">IF(AND(ISBLANK(F91),ISBLANK(G91),ISBLANK(H91)), E91, _xlfn.CONCAT(E91,"--",_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(ISBLANK(F91),"",_xlfn.CONCAT(F91,"-")),IF(ISBLANK(G91),"",_xlfn.CONCAT(G91,"-")),IF(ISBLANK(H91),"",_xlfn.CONCAT(H91,"-"))),IF(_xlpm.X="","",LEFT(_xlpm.X,LEN(_xlpm.X)-1)))))</f>
@@ -45071,10 +45134,10 @@
         <v>oceano</v>
       </c>
       <c r="F91" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="G91" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="P91">
         <v>1</v>
@@ -45117,13 +45180,13 @@
         <v>oceano</v>
       </c>
       <c r="F93" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="H93" t="s">
-        <v>2957</v>
+        <v>2956</v>
       </c>
       <c r="I93" t="s">
-        <v>2950</v>
+        <v>2949</v>
       </c>
       <c r="P93">
         <v>1</v>
@@ -45146,10 +45209,10 @@
         <v>oceano</v>
       </c>
       <c r="F94" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H94" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="P94">
         <v>1</v>
@@ -45172,10 +45235,10 @@
         <v>oceano</v>
       </c>
       <c r="F95" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G95" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
       <c r="I95" s="7" t="s">
         <v>1245</v>
@@ -45201,7 +45264,7 @@
         <v>oceano</v>
       </c>
       <c r="F96" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="P96">
         <v>1</v>
@@ -45224,10 +45287,10 @@
         <v>oceano</v>
       </c>
       <c r="F97" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H97" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="P97">
         <v>1</v>
@@ -45250,10 +45313,10 @@
         <v>oceano</v>
       </c>
       <c r="F98" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G98" t="s">
-        <v>2962</v>
+        <v>2961</v>
       </c>
       <c r="P98">
         <v>1</v>
@@ -45305,7 +45368,7 @@
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="8"/>
@@ -45336,10 +45399,10 @@
         <v>oceano</v>
       </c>
       <c r="F102" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="G102" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="P102">
         <v>1</v>
@@ -45759,6 +45822,9 @@
       <c r="A123" s="5" t="s">
         <v>1054</v>
       </c>
+      <c r="B123" t="s">
+        <v>3010</v>
+      </c>
       <c r="D123" t="str">
         <f t="shared" si="8"/>
         <v>maré--motivo</v>
@@ -45768,7 +45834,7 @@
         <v>maré</v>
       </c>
       <c r="F123" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="R123">
         <v>1</v>
@@ -45791,10 +45857,10 @@
         <v>outras</v>
       </c>
       <c r="F124" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G124" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
       <c r="AD124">
         <v>1</v>
@@ -45808,6 +45874,9 @@
       <c r="A125" s="5" t="s">
         <v>1833</v>
       </c>
+      <c r="B125" t="s">
+        <v>3008</v>
+      </c>
       <c r="D125" t="str">
         <f t="shared" si="8"/>
         <v>maré</v>
@@ -45828,6 +45897,9 @@
       <c r="A126" s="5" t="s">
         <v>1140</v>
       </c>
+      <c r="B126" t="s">
+        <v>3009</v>
+      </c>
       <c r="D126" t="str">
         <f t="shared" si="8"/>
         <v>maré</v>
@@ -45848,14 +45920,29 @@
       <c r="A127" s="7" t="s">
         <v>1279</v>
       </c>
+      <c r="B127" t="s">
+        <v>3006</v>
+      </c>
+      <c r="C127" t="s">
+        <v>3005</v>
+      </c>
       <c r="D127" t="str">
         <f t="shared" si="8"/>
-        <v>maré</v>
+        <v>maré--detalhar-frequência</v>
       </c>
       <c r="E127" t="str">
         <f t="shared" si="9"/>
         <v>maré</v>
       </c>
+      <c r="F127" t="s">
+        <v>2876</v>
+      </c>
+      <c r="G127" t="s">
+        <v>3001</v>
+      </c>
+      <c r="I127" t="s">
+        <v>3007</v>
+      </c>
       <c r="R127">
         <v>1</v>
       </c>
@@ -45868,6 +45955,12 @@
       <c r="A128" s="7" t="s">
         <v>2672</v>
       </c>
+      <c r="B128" t="s">
+        <v>3002</v>
+      </c>
+      <c r="C128" t="s">
+        <v>3005</v>
+      </c>
       <c r="D128" t="str">
         <f t="shared" si="8"/>
         <v>maré</v>
@@ -45888,6 +45981,12 @@
       <c r="A129" s="7" t="s">
         <v>1488</v>
       </c>
+      <c r="B129" t="s">
+        <v>3003</v>
+      </c>
+      <c r="C129" t="s">
+        <v>3005</v>
+      </c>
       <c r="D129" t="str">
         <f t="shared" si="8"/>
         <v>maré</v>
@@ -45908,6 +46007,12 @@
       <c r="A130" s="7" t="s">
         <v>1552</v>
       </c>
+      <c r="B130" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C130" t="s">
+        <v>3005</v>
+      </c>
       <c r="D130" t="str">
         <f t="shared" si="8"/>
         <v>maré</v>
@@ -45930,12 +46035,15 @@
       </c>
       <c r="D131" t="str">
         <f t="shared" ref="D131:D194" si="13">IF(AND(ISBLANK(F131),ISBLANK(G131),ISBLANK(H131)), E131, _xlfn.CONCAT(E131,"--",_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(ISBLANK(F131),"",_xlfn.CONCAT(F131,"-")),IF(ISBLANK(G131),"",_xlfn.CONCAT(G131,"-")),IF(ISBLANK(H131),"",_xlfn.CONCAT(H131,"-"))),IF(_xlpm.X="","",LEFT(_xlpm.X,LEN(_xlpm.X)-1)))))</f>
-        <v>corrente</v>
+        <v>corrente--listar</v>
       </c>
       <c r="E131" t="str">
         <f t="shared" ref="E131:E194" si="14">_xlfn.LET(_xlpm.X,_xlfn.CONCAT(IF(J131=1, _xlfn.CONCAT(J$1,"-"), ""), IF(K131=1, _xlfn.CONCAT(K$1,"-"), ""),IF(L131=1, _xlfn.CONCAT(L$1,"-"), ""),IF(M131=1, _xlfn.CONCAT(M$1,"-"), ""),IF(N131=1, _xlfn.CONCAT(N$1,"-"), ""),IF(O131=1, _xlfn.CONCAT(O$1,"-"), ""),IF(P131=1, _xlfn.CONCAT(P$1,"-"), ""),IF(Q131=1, _xlfn.CONCAT(Q$1,"-"), ""),IF(R131=1, _xlfn.CONCAT(R$1,"-"), ""),IF(S131=1, _xlfn.CONCAT(S$1,"-"), ""),IF(T131=1, _xlfn.CONCAT(T$1,"-"), ""),IF(U131=1, _xlfn.CONCAT(U$1,"-"), ""),IF(V131=1, _xlfn.CONCAT(V$1,"-"), ""),IF(W131=1, _xlfn.CONCAT(W$1,"-"), ""),IF(X131=1, _xlfn.CONCAT(X$1,"-"), ""),IF(Y131=1, _xlfn.CONCAT(Y$1,"-"), ""),IF(Z131=1, _xlfn.CONCAT(Z$1,"-"), ""),IF(AA131=1, _xlfn.CONCAT(AA$1,"-"), ""),IF(AB131=1, _xlfn.CONCAT(AB$1,"-"), ""),IF(AC131=1, _xlfn.CONCAT(AC$1,"-"), ""),IF(AD131=1, _xlfn.CONCAT(AD$1,"-"), "")),LEFT(_xlpm.X,LEN(_xlpm.X)-1))</f>
         <v>corrente</v>
       </c>
+      <c r="F131" t="s">
+        <v>2837</v>
+      </c>
       <c r="S131">
         <v>1</v>
       </c>
@@ -45968,14 +46076,20 @@
       <c r="A133" s="7" t="s">
         <v>2621</v>
       </c>
+      <c r="B133" t="s">
+        <v>3011</v>
+      </c>
       <c r="D133" t="str">
         <f t="shared" si="13"/>
-        <v>corrente</v>
+        <v>corrente--definição</v>
       </c>
       <c r="E133" t="str">
         <f t="shared" si="14"/>
         <v>corrente</v>
       </c>
+      <c r="F133" t="s">
+        <v>2958</v>
+      </c>
       <c r="S133">
         <v>1</v>
       </c>
@@ -45990,12 +46104,18 @@
       </c>
       <c r="D134" t="str">
         <f t="shared" si="13"/>
-        <v>corrente</v>
+        <v>corrente--motivo</v>
       </c>
       <c r="E134" t="str">
         <f t="shared" si="14"/>
         <v>corrente</v>
       </c>
+      <c r="F134" t="s">
+        <v>2856</v>
+      </c>
+      <c r="I134" t="s">
+        <v>3012</v>
+      </c>
       <c r="S134">
         <v>1</v>
       </c>
@@ -46135,10 +46255,10 @@
         <v>2706</v>
       </c>
       <c r="B141" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
       <c r="C141" t="s">
-        <v>2817</v>
+        <v>2816</v>
       </c>
       <c r="D141" t="str">
         <f t="shared" si="13"/>
@@ -46149,10 +46269,10 @@
         <v>flora</v>
       </c>
       <c r="F141" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G141" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="U141">
         <v>1</v>
@@ -46164,13 +46284,13 @@
     </row>
     <row r="142" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="B142" t="s">
+        <v>2817</v>
+      </c>
+      <c r="C142" t="s">
         <v>2818</v>
-      </c>
-      <c r="C142" t="s">
-        <v>2819</v>
       </c>
       <c r="D142" t="str">
         <f t="shared" si="13"/>
@@ -46181,10 +46301,10 @@
         <v>flora-fauna</v>
       </c>
       <c r="F142" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G142" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="U142">
         <v>1</v>
@@ -46199,13 +46319,13 @@
     </row>
     <row r="143" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
+        <v>2813</v>
+      </c>
+      <c r="B143" t="s">
+        <v>2815</v>
+      </c>
+      <c r="C143" t="s">
         <v>2814</v>
-      </c>
-      <c r="B143" t="s">
-        <v>2816</v>
-      </c>
-      <c r="C143" t="s">
-        <v>2815</v>
       </c>
       <c r="D143" t="str">
         <f t="shared" si="13"/>
@@ -46216,10 +46336,10 @@
         <v>flora-fauna</v>
       </c>
       <c r="F143" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G143" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="U143">
         <v>1</v>
@@ -46251,10 +46371,10 @@
         <v>fauna</v>
       </c>
       <c r="F144" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G144" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="V144">
         <v>1</v>
@@ -46283,10 +46403,10 @@
         <v>coral</v>
       </c>
       <c r="F145" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H145" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="J145">
         <v>1</v>
@@ -46312,10 +46432,10 @@
         <v>fauna</v>
       </c>
       <c r="F146" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G146" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="V146">
         <v>1</v>
@@ -46341,10 +46461,10 @@
         <v>fauna</v>
       </c>
       <c r="F147" t="s">
+        <v>2958</v>
+      </c>
+      <c r="G147" t="s">
         <v>2959</v>
-      </c>
-      <c r="G147" t="s">
-        <v>2960</v>
       </c>
       <c r="V147">
         <v>1</v>
@@ -46370,13 +46490,13 @@
         <v>fauna</v>
       </c>
       <c r="F148" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G148" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="H148" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="V148">
         <v>1</v>
@@ -46405,10 +46525,10 @@
         <v>fauna</v>
       </c>
       <c r="F149" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G149" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="V149">
         <v>1</v>
@@ -46437,10 +46557,10 @@
         <v>fauna</v>
       </c>
       <c r="F150" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G150" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="V150">
         <v>1</v>
@@ -46455,7 +46575,7 @@
         <v>2799</v>
       </c>
       <c r="B151" t="s">
-        <v>2805</v>
+        <v>2999</v>
       </c>
       <c r="C151" t="s">
         <v>2801</v>
@@ -46469,10 +46589,10 @@
         <v>fauna</v>
       </c>
       <c r="F151" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G151" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="V151">
         <v>1</v>
@@ -46484,7 +46604,10 @@
     </row>
     <row r="152" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
-        <v>2882</v>
+        <v>2881</v>
+      </c>
+      <c r="B152" t="s">
+        <v>3000</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="13"/>
@@ -46495,13 +46618,13 @@
         <v>fauna</v>
       </c>
       <c r="F152" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="G152" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="H152" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="V152">
         <v>1</v>
@@ -46516,10 +46639,10 @@
         <v>2679</v>
       </c>
       <c r="B153" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="C153" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="D153" t="str">
         <f t="shared" si="13"/>
@@ -46530,13 +46653,13 @@
         <v>fauna</v>
       </c>
       <c r="F153" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="G153" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="H153" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="V153">
         <v>1</v>
@@ -46548,10 +46671,10 @@
     </row>
     <row r="154" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="B154" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="D154" t="str">
         <f t="shared" si="13"/>
@@ -46562,10 +46685,10 @@
         <v>fauna</v>
       </c>
       <c r="F154" t="s">
+        <v>2868</v>
+      </c>
+      <c r="G154" t="s">
         <v>2869</v>
-      </c>
-      <c r="G154" t="s">
-        <v>2870</v>
       </c>
       <c r="V154">
         <v>1</v>
@@ -46577,13 +46700,13 @@
     </row>
     <row r="155" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
+        <v>2809</v>
+      </c>
+      <c r="B155" t="s">
+        <v>2811</v>
+      </c>
+      <c r="C155" t="s">
         <v>2810</v>
-      </c>
-      <c r="B155" t="s">
-        <v>2812</v>
-      </c>
-      <c r="C155" t="s">
-        <v>2811</v>
       </c>
       <c r="D155" t="str">
         <f t="shared" si="13"/>
@@ -46594,10 +46717,10 @@
         <v>fauna-turismo</v>
       </c>
       <c r="F155" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="G155" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="V155">
         <v>1</v>
@@ -46675,7 +46798,7 @@
         <v>2683</v>
       </c>
       <c r="B159" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="C159" t="s">
         <v>2755</v>
@@ -46689,10 +46812,10 @@
         <v>fauna</v>
       </c>
       <c r="F159" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G159" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="V159">
         <v>1</v>
@@ -46707,7 +46830,7 @@
         <v>2768</v>
       </c>
       <c r="B160" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="C160" t="s">
         <v>2770</v>
@@ -46721,10 +46844,10 @@
         <v>fauna</v>
       </c>
       <c r="F160" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G160" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="V160">
         <v>1</v>
@@ -46750,10 +46873,10 @@
         <v>fauna</v>
       </c>
       <c r="F161" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G161" t="s">
-        <v>2864</v>
+        <v>2863</v>
       </c>
       <c r="V161">
         <v>1</v>
@@ -46768,7 +46891,7 @@
         <v>2769</v>
       </c>
       <c r="B162" t="s">
-        <v>2829</v>
+        <v>2828</v>
       </c>
       <c r="C162" t="s">
         <v>2771</v>
@@ -46782,10 +46905,10 @@
         <v>fauna</v>
       </c>
       <c r="F162" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G162" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
       <c r="V162">
         <v>1</v>
@@ -46814,10 +46937,10 @@
         <v>fauna</v>
       </c>
       <c r="F163" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G163" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
       <c r="V163">
         <v>1</v>
@@ -46843,10 +46966,10 @@
         <v>fauna</v>
       </c>
       <c r="F164" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G164" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="V164">
         <v>1</v>
@@ -46875,10 +46998,10 @@
         <v>fauna-turismo</v>
       </c>
       <c r="F165" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="G165" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="V165">
         <v>1</v>
@@ -46927,10 +47050,10 @@
         <v>fauna</v>
       </c>
       <c r="F167" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G167" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="V167">
         <v>1</v>
@@ -46959,10 +47082,10 @@
         <v>fauna</v>
       </c>
       <c r="F168" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G168" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="V168">
         <v>1</v>
@@ -46988,10 +47111,10 @@
         <v>fauna</v>
       </c>
       <c r="F169" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G169" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="V169">
         <v>1</v>
@@ -47017,10 +47140,10 @@
         <v>fauna</v>
       </c>
       <c r="F170" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G170" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="V170">
         <v>1</v>
@@ -47069,10 +47192,10 @@
         <v>fauna</v>
       </c>
       <c r="F172" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G172" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="V172">
         <v>1</v>
@@ -47098,10 +47221,10 @@
         <v>fauna</v>
       </c>
       <c r="F173" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="G173" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="V173">
         <v>1</v>
@@ -47130,10 +47253,10 @@
         <v>fauna</v>
       </c>
       <c r="F174" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G174" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="V174">
         <v>1</v>
@@ -47162,13 +47285,13 @@
         <v>fauna</v>
       </c>
       <c r="F175" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G175" t="s">
+        <v>2877</v>
+      </c>
+      <c r="I175" t="s">
         <v>2878</v>
-      </c>
-      <c r="I175" t="s">
-        <v>2879</v>
       </c>
       <c r="V175">
         <v>1</v>
@@ -47197,10 +47320,10 @@
         <v>fauna</v>
       </c>
       <c r="F176" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G176" t="s">
-        <v>2961</v>
+        <v>2960</v>
       </c>
       <c r="V176">
         <v>1</v>
@@ -47215,7 +47338,7 @@
         <v>2759</v>
       </c>
       <c r="B177" t="s">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="C177" t="s">
         <v>2760</v>
@@ -47229,13 +47352,13 @@
         <v>fauna</v>
       </c>
       <c r="F177" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="G177" t="s">
-        <v>2876</v>
+        <v>2875</v>
       </c>
       <c r="I177" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="V177">
         <v>1</v>
@@ -47261,10 +47384,10 @@
         <v>fauna</v>
       </c>
       <c r="F178" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G178" t="s">
-        <v>2961</v>
+        <v>2960</v>
       </c>
       <c r="V178">
         <v>1</v>
@@ -47853,10 +47976,10 @@
         <v>gás</v>
       </c>
       <c r="F207" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="H207" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="M207">
         <v>1</v>
@@ -47879,13 +48002,13 @@
         <v>outras</v>
       </c>
       <c r="F208" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G208" t="s">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="H208" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="AD208">
         <v>1</v>
@@ -47914,13 +48037,13 @@
         <v>outras</v>
       </c>
       <c r="F209" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="G209" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="H209" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="AD209">
         <v>1</v>
@@ -47949,13 +48072,13 @@
         <v>outras</v>
       </c>
       <c r="F210" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="G210" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="H210" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="AD210">
         <v>1</v>

</xml_diff>

<commit_message>
move unit tests before saving file
</commit_message>
<xml_diff>
--- a/results/Perguntas.xlsx
+++ b/results/Perguntas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\Python\Filter-MSMARCO\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D21821-3977-4234-A4FB-26F2A220D936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F29980-8AE8-4023-9CF9-D8840CC53A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="565" firstSheet="2" activeTab="3" xr2:uid="{90144E09-7748-454D-AFCB-3F2406963FB8}"/>
   </bookViews>
@@ -43381,10 +43381,10 @@
   <dimension ref="A1:AH529"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G152" sqref="G152"/>
+      <selection pane="bottomRight" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43580,7 +43580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3021</v>
       </c>
@@ -43612,7 +43612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>2593</v>
       </c>
@@ -43647,7 +43647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>2594</v>
       </c>
@@ -43679,7 +43679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>2595</v>
       </c>
@@ -43705,7 +43705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>2596</v>
       </c>
@@ -43731,7 +43731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>2597</v>
       </c>
@@ -43760,7 +43760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>2898</v>
       </c>
@@ -43789,7 +43789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>2598</v>
       </c>
@@ -43821,7 +43821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2903</v>
       </c>
@@ -43856,7 +43856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>2599</v>
       </c>
@@ -43891,7 +43891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>2600</v>
       </c>
@@ -43923,7 +43923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>2601</v>
       </c>
@@ -43958,7 +43958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>3282</v>
       </c>
@@ -43990,7 +43990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>2602</v>
       </c>
@@ -44022,7 +44022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>2603</v>
       </c>
@@ -44054,7 +44054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>2910</v>
       </c>
@@ -44083,7 +44083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1027</v>
       </c>
@@ -44115,7 +44115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2745</v>
       </c>
@@ -44147,7 +44147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>3018</v>
       </c>
@@ -44179,7 +44179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>2922</v>
       </c>
@@ -44208,7 +44208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>2842</v>
       </c>
@@ -44240,7 +44240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>2843</v>
       </c>
@@ -44272,7 +44272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>2907</v>
       </c>
@@ -44304,7 +44304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>2604</v>
       </c>
@@ -44333,7 +44333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>2916</v>
       </c>
@@ -44365,7 +44365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>2844</v>
       </c>
@@ -44423,7 +44423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>2605</v>
       </c>
@@ -44455,7 +44455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>2606</v>
       </c>
@@ -44490,7 +44490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>2607</v>
       </c>
@@ -44522,7 +44522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>2039</v>
       </c>
@@ -44554,7 +44554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>2947</v>
       </c>
@@ -44616,7 +44616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>2735</v>
       </c>
@@ -44648,7 +44648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>2965</v>
       </c>
@@ -44683,7 +44683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2608</v>
       </c>
@@ -44715,7 +44715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>2962</v>
       </c>
@@ -44747,7 +44747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>2609</v>
       </c>
@@ -44779,7 +44779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>2989</v>
       </c>
@@ -44811,7 +44811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>2821</v>
       </c>
@@ -44843,7 +44843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>2731</v>
       </c>
@@ -44875,7 +44875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>2728</v>
       </c>
@@ -44907,7 +44907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>2610</v>
       </c>
@@ -44939,7 +44939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>2611</v>
       </c>
@@ -44971,7 +44971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2612</v>
       </c>
@@ -45000,7 +45000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>2957</v>
       </c>
@@ -45032,7 +45032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>1626</v>
       </c>
@@ -45090,7 +45090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>1559</v>
       </c>
@@ -45119,7 +45119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>2615</v>
       </c>
@@ -45177,7 +45177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>2617</v>
       </c>
@@ -45203,7 +45203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>2618</v>
       </c>
@@ -45229,7 +45229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>2970</v>
       </c>
@@ -45284,7 +45284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>2724</v>
       </c>
@@ -45446,7 +45446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>2727</v>
       </c>
@@ -45478,7 +45478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>2732</v>
       </c>
@@ -45507,7 +45507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>2640</v>
       </c>
@@ -45641,7 +45641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>2574</v>
       </c>
@@ -45699,7 +45699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>2576</v>
       </c>
@@ -45731,7 +45731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>3281</v>
       </c>
@@ -45763,7 +45763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>2577</v>
       </c>
@@ -45792,7 +45792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>2765</v>
       </c>
@@ -45821,7 +45821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>2767</v>
       </c>
@@ -45850,7 +45850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>2578</v>
       </c>
@@ -45879,7 +45879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
         <v>2579</v>
       </c>
@@ -45908,7 +45908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>2580</v>
       </c>
@@ -45960,7 +45960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
         <v>2583</v>
       </c>
@@ -45989,7 +45989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>2584</v>
       </c>
@@ -46021,7 +46021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>2585</v>
       </c>
@@ -46053,7 +46053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
         <v>2586</v>
       </c>
@@ -46082,7 +46082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>2587</v>
       </c>
@@ -46163,7 +46163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
         <v>2590</v>
       </c>
@@ -46189,7 +46189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
         <v>2591</v>
       </c>
@@ -46248,7 +46248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
         <v>2592</v>
       </c>
@@ -46281,7 +46281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
         <v>2643</v>
       </c>
@@ -46627,7 +46627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
         <v>3278</v>
       </c>
@@ -46659,7 +46659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
         <v>2629</v>
       </c>
@@ -46694,7 +46694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>1582</v>
       </c>
@@ -46727,7 +46727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A109" s="7" t="s">
         <v>2894</v>
       </c>
@@ -47420,7 +47420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A140" s="7" t="s">
         <v>3035</v>
       </c>
@@ -47452,7 +47452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>3161</v>
       </c>
@@ -47484,7 +47484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>1833</v>
       </c>
@@ -47516,7 +47516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
         <v>1279</v>
       </c>
@@ -47551,7 +47551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A144" s="7" t="s">
         <v>2669</v>
       </c>
@@ -47583,7 +47583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A145" s="7" t="s">
         <v>1488</v>
       </c>
@@ -47615,7 +47615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A146" s="7" t="s">
         <v>1552</v>
       </c>
@@ -47719,7 +47719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A150" s="7" t="s">
         <v>2619</v>
       </c>
@@ -47902,7 +47902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A156" s="7" t="s">
         <v>2771</v>
       </c>
@@ -47928,7 +47928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A157" s="7" t="s">
         <v>2770</v>
       </c>
@@ -47954,7 +47954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A158" s="7" t="s">
         <v>2674</v>
       </c>
@@ -48087,7 +48087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A163" s="7" t="s">
         <v>3197</v>
       </c>
@@ -48116,7 +48116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A164" s="7" t="s">
         <v>3202</v>
       </c>
@@ -48148,7 +48148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A165" s="7" t="s">
         <v>3024</v>
       </c>
@@ -48186,7 +48186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A166" s="7" t="s">
         <v>3196</v>
       </c>
@@ -48218,7 +48218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A167" s="7" t="s">
         <v>3023</v>
       </c>
@@ -48250,7 +48250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A168" s="7" t="s">
         <v>3199</v>
       </c>
@@ -48285,7 +48285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A169" s="7" t="s">
         <v>3237</v>
       </c>
@@ -48317,7 +48317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
         <v>3217</v>
       </c>
@@ -48349,7 +48349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A171" s="7" t="s">
         <v>3230</v>
       </c>
@@ -48427,7 +48427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
         <v>2788</v>
       </c>
@@ -48462,7 +48462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A175" s="7" t="s">
         <v>2789</v>
       </c>
@@ -48537,7 +48537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A178" s="7" t="s">
         <v>2698</v>
       </c>
@@ -48569,7 +48569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A179" s="7" t="s">
         <v>2754</v>
       </c>
@@ -48601,7 +48601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A180" s="7" t="s">
         <v>2758</v>
       </c>
@@ -48630,7 +48630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A181" s="7" t="s">
         <v>2773</v>
       </c>
@@ -48662,7 +48662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A182" s="7" t="s">
         <v>2774</v>
       </c>
@@ -48694,7 +48694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A183" s="7" t="s">
         <v>2775</v>
       </c>
@@ -48726,7 +48726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A184" s="7" t="s">
         <v>2841</v>
       </c>
@@ -48761,7 +48761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A185" s="7" t="s">
         <v>3247</v>
       </c>
@@ -48822,7 +48822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
         <v>2678</v>
       </c>
@@ -48854,7 +48854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A188" s="7" t="s">
         <v>2748</v>
       </c>
@@ -48886,7 +48886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A189" s="7" t="s">
         <v>2752</v>
       </c>
@@ -48915,7 +48915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A190" s="7" t="s">
         <v>2749</v>
       </c>
@@ -48947,7 +48947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A191" s="7" t="s">
         <v>2679</v>
       </c>
@@ -48979,7 +48979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A192" s="7" t="s">
         <v>2760</v>
       </c>
@@ -49008,7 +49008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
         <v>2680</v>
       </c>
@@ -49043,7 +49043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A194" s="7" t="s">
         <v>2695</v>
       </c>
@@ -49072,7 +49072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
         <v>2696</v>
       </c>
@@ -49104,7 +49104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>2697</v>
       </c>
@@ -49133,7 +49133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>2699</v>
       </c>
@@ -49162,7 +49162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
         <v>2694</v>
       </c>
@@ -49194,7 +49194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
         <v>2712</v>
       </c>
@@ -49226,7 +49226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
         <v>2716</v>
       </c>
@@ -49258,7 +49258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A201" s="7" t="s">
         <v>2717</v>
       </c>
@@ -49293,7 +49293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
         <v>2738</v>
       </c>
@@ -49328,7 +49328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A203" s="7" t="s">
         <v>2740</v>
       </c>
@@ -49363,7 +49363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A204" s="7" t="s">
         <v>2743</v>
       </c>
@@ -49392,7 +49392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A205" s="7" t="s">
         <v>2973</v>
       </c>
@@ -49424,7 +49424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A206" s="7" t="s">
         <v>3032</v>
       </c>
@@ -49456,7 +49456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A207" s="7" t="s">
         <v>3130</v>
       </c>
@@ -49491,7 +49491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A208" s="7" t="s">
         <v>3137</v>
       </c>
@@ -49523,7 +49523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A209" s="7" t="s">
         <v>3138</v>
       </c>
@@ -49555,7 +49555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A210" s="7" t="s">
         <v>3140</v>
       </c>
@@ -49587,7 +49587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A211" s="7" t="s">
         <v>3148</v>
       </c>
@@ -49619,7 +49619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A212" s="7" t="s">
         <v>2785</v>
       </c>
@@ -49654,7 +49654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
         <v>2782</v>
       </c>
@@ -49683,7 +49683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A214" s="7" t="s">
         <v>3017</v>
       </c>
@@ -49712,7 +49712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A215" s="7" t="s">
         <v>3182</v>
       </c>
@@ -49741,7 +49741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A216" s="7" t="s">
         <v>3139</v>
       </c>
@@ -50039,7 +50039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A227" s="7" t="s">
         <v>3284</v>
       </c>
@@ -50111,7 +50111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A230" s="7" t="s">
         <v>3299</v>
       </c>
@@ -50140,7 +50140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A231" s="7" t="s">
         <v>2710</v>
       </c>
@@ -50175,7 +50175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A232" s="7" t="s">
         <v>2635</v>
       </c>
@@ -50207,7 +50207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A233" s="7" t="s">
         <v>2638</v>
       </c>
@@ -50239,7 +50239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A234" s="7" t="s">
         <v>3208</v>
       </c>
@@ -50271,7 +50271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A235" s="7" t="s">
         <v>2641</v>
       </c>
@@ -50303,7 +50303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A236" s="7" t="s">
         <v>2642</v>
       </c>
@@ -50335,7 +50335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A237" s="7" t="s">
         <v>3242</v>
       </c>
@@ -50393,7 +50393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A239" s="7" t="s">
         <v>2708</v>
       </c>
@@ -50425,7 +50425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A240" s="7" t="s">
         <v>3233</v>
       </c>
@@ -50457,7 +50457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A241" s="7" t="s">
         <v>2709</v>
       </c>
@@ -50489,7 +50489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A242" s="7" t="s">
         <v>3028</v>
       </c>
@@ -50521,7 +50521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A243" s="7" t="s">
         <v>3068</v>
       </c>
@@ -50579,7 +50579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A245" s="7" t="s">
         <v>3171</v>
       </c>
@@ -50611,7 +50611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A246" s="7" t="s">
         <v>2637</v>
       </c>
@@ -50643,7 +50643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A247" s="7" t="s">
         <v>2636</v>
       </c>
@@ -50678,7 +50678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A248" s="7" t="s">
         <v>3167</v>
       </c>
@@ -50713,7 +50713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A249" s="7" t="s">
         <v>3074</v>
       </c>
@@ -50745,7 +50745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A250" s="7" t="s">
         <v>3077</v>
       </c>
@@ -50780,7 +50780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A251" s="7" t="s">
         <v>2639</v>
       </c>
@@ -50812,7 +50812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A252" s="7" t="s">
         <v>3173</v>
       </c>
@@ -50844,7 +50844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A253" s="7" t="s">
         <v>3178</v>
       </c>
@@ -50876,7 +50876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A254" s="7" t="s">
         <v>3190</v>
       </c>
@@ -50908,7 +50908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A255" s="7" t="s">
         <v>3071</v>
       </c>
@@ -50940,7 +50940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A256" s="7" t="s">
         <v>3082</v>
       </c>
@@ -50972,7 +50972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A257" s="7" t="s">
         <v>3083</v>
       </c>
@@ -51004,7 +51004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A258" s="7" t="s">
         <v>3084</v>
       </c>
@@ -51239,7 +51239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A266" s="7" t="s">
         <v>3105</v>
       </c>
@@ -51271,7 +51271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A267" s="7" t="s">
         <v>3111</v>
       </c>
@@ -51306,7 +51306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A268" s="7" t="s">
         <v>3109</v>
       </c>
@@ -51341,7 +51341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A269" s="7" t="s">
         <v>3112</v>
       </c>
@@ -51373,7 +51373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A270" s="7" t="s">
         <v>3113</v>
       </c>
@@ -51408,7 +51408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A271" s="7" t="s">
         <v>3114</v>
       </c>
@@ -51440,7 +51440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A272" s="7" t="s">
         <v>3115</v>
       </c>
@@ -51472,7 +51472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A273" s="7" t="s">
         <v>3262</v>
       </c>
@@ -53968,11 +53968,6 @@
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="extinção"/>
-      </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH529">
       <sortCondition descending="1" ref="J2:J529"/>
@@ -54060,7 +54055,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adições finais de intents
</commit_message>
<xml_diff>
--- a/results/Perguntas.xlsx
+++ b/results/Perguntas.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10595" uniqueCount="3912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10596" uniqueCount="3913">
   <si>
     <t>query</t>
   </si>
@@ -11910,6 +11910,9 @@
   </si>
   <si>
     <t>mero</t>
+  </si>
+  <si>
+    <t>Quais são as melhores praias?</t>
   </si>
 </sst>
 </file>
@@ -45430,11 +45433,11 @@
   <dimension ref="A1:AH492"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B378" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B189" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B385" sqref="B385"/>
       <selection pane="topRight" activeCell="B385" sqref="B385"/>
       <selection pane="bottomLeft" activeCell="B385" sqref="B385"/>
-      <selection pane="bottomRight" activeCell="D399" sqref="D399"/>
+      <selection pane="bottomRight" activeCell="I217" sqref="I217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52351,6 +52354,9 @@
       </c>
       <c r="G217" t="s">
         <v>3051</v>
+      </c>
+      <c r="I217" t="s">
+        <v>3912</v>
       </c>
       <c r="Z217">
         <v>1</v>

</xml_diff>